<commit_message>
updates to test visualization
</commit_message>
<xml_diff>
--- a/visualization_wip.xlsx
+++ b/visualization_wip.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60E3C066-C2B1-40FF-A505-0189C8D8ED25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E95F18-B512-4889-851B-ECFE31001B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="533" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -151,19 +151,6 @@
       <top style="thin">
         <color indexed="21"/>
       </top>
-      <bottom style="thin">
-        <color indexed="21"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="21"/>
-      </left>
-      <right style="thin">
-        <color indexed="21"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="21"/>
       </bottom>
@@ -201,11 +188,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -221,19 +208,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="2">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="2">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -489,13 +473,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2045460</xdr:colOff>
+      <xdr:colOff>2079170</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>245370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1219199</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>231954</xdr:rowOff>
     </xdr:to>
@@ -517,8 +501,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5376489" y="746113"/>
-          <a:ext cx="1296454" cy="1989555"/>
+          <a:off x="5410199" y="746113"/>
+          <a:ext cx="1262743" cy="1989555"/>
           <a:chOff x="460" y="254"/>
           <a:chExt cx="69" cy="408"/>
         </a:xfrm>
@@ -909,7 +893,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm flipH="1">
-            <a:off x="655" y="1087"/>
+            <a:off x="655" y="1055"/>
             <a:ext cx="41" cy="0"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -1270,7 +1254,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="364" y="265"/>
+            <a:off x="364" y="284"/>
             <a:ext cx="31" cy="0"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -3075,24 +3059,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="82.109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="2.77734375" style="10" customWidth="1"/>
-    <col min="4" max="16384" width="8.77734375" style="10"/>
+    <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="82.109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="2.77734375" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.77734375" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3111,7 +3095,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.88671875" defaultRowHeight="39.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3132,35 +3116,76 @@
       <c r="A1" s="4">
         <v>1</v>
       </c>
-      <c r="K1" s="4"/>
+      <c r="C1" s="3" t="b">
+        <f ca="1">AND(C2=1,C6=3)</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="3">
+        <f ca="1">IF(C1=TRUE,'Win probabilities'!A3)</f>
+        <v>0.50636093869825483</v>
+      </c>
+      <c r="K1" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="3">
+        <f>'Win probabilities'!A2</f>
+        <v>0.98278630377518839</v>
+      </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6">
-        <f ca="1">IF(RAND()&gt;'Win probabilities'!C2,Tournament!A1,Tournament!A3)</f>
-        <v>2</v>
-      </c>
-      <c r="I2" s="7"/>
+        <f ca="1">IF(RAND()&lt;A2,A1,A3)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="C3" s="3" t="b">
+        <f ca="1">AND(C2=2,C6=3)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="b">
+        <f ca="1">IF(C3=TRUE,'Win probabilities'!B3)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="E4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="E4" s="7">
+        <f ca="1">IF(RAND()&lt;SUM(D1:D7),C2,C6)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="C5" s="3" t="b">
+        <f ca="1">AND(C2=1,C6=4)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="b">
+        <f ca="1">IF(C5=TRUE,'Win probabilities'!A4)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="3">
+        <f>'Win probabilities'!C4</f>
+        <v>0.60284487256253583</v>
+      </c>
       <c r="C6" s="6">
-        <f ca="1">IF(RAND()&gt;'Win probabilities'!E4,Tournament!A5,Tournament!A7)</f>
+        <f ca="1">IF(RAND()&lt;A6,A5,A7)</f>
         <v>3</v>
       </c>
       <c r="I6" s="6"/>
@@ -3169,41 +3194,116 @@
       <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="K7" s="4"/>
+      <c r="C7" s="3" t="b">
+        <f ca="1">AND(C2=2,C6=4)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="b">
+        <f ca="1">IF(C7=TRUE,'Win probabilities'!B4)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="F8" s="9"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="A9" s="4">
+        <v>5</v>
+      </c>
+      <c r="K9" s="4">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="F10" s="9"/>
+      <c r="A10" s="3">
+        <f>'Win probabilities'!E6</f>
+        <v>0.99337376369869701</v>
+      </c>
+      <c r="C10" s="3" t="b">
+        <f ca="1">AND(C11=5,C15=7)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <f ca="1">IF(C10=TRUE,'Win probabilities'!E7)</f>
+        <v>0.27960125734444374</v>
+      </c>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="C11" s="6"/>
+      <c r="C11" s="6">
+        <f ca="1">IF(RAND()&lt;A10,A9,A12)</f>
+        <v>5</v>
+      </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="A12" s="4">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="b">
+        <f ca="1">AND(C11=6,C15=7)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="b">
+        <f ca="1">IF(C12=TRUE,'Win probabilities'!F7)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="E13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="E13" s="7">
+        <f ca="1">IF(RAND()&lt;SUM(D10:D16),C11,C15)</f>
+        <v>7</v>
+      </c>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="A14" s="4">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="b">
+        <f ca="1">AND(C11=5,C15=8)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="b">
+        <f ca="1">IF(C14=TRUE,'Win probabilities'!E8)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="C15" s="6"/>
+      <c r="A15" s="3">
+        <f>'Win probabilities'!G8</f>
+        <v>0.18390650213337789</v>
+      </c>
+      <c r="C15" s="6">
+        <f ca="1">IF(RAND()&lt;A15,A14,A16)</f>
+        <v>7</v>
+      </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="A16" s="4">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="b">
+        <f ca="1">AND(C11=6,C15=8)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="b">
+        <f ca="1">IF(C16=TRUE,'Win probabilities'!F8)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="18" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3220,909 +3320,811 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945F8664-1F88-4A49-B797-31F1E9DFD72F}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
       <c r="B1">
-        <v>1</v>
+        <v>0.98278630377518839</v>
       </c>
       <c r="C1">
-        <v>2</v>
+        <v>0.50636093869825483</v>
       </c>
       <c r="D1">
-        <v>3</v>
+        <v>0.73397479367659013</v>
       </c>
       <c r="E1">
-        <v>4</v>
+        <v>0.88924777405780919</v>
       </c>
       <c r="F1">
-        <v>5</v>
+        <v>0.69153678025465826</v>
       </c>
       <c r="G1">
-        <v>6</v>
+        <v>0.62990478407748318</v>
       </c>
       <c r="H1">
-        <v>7</v>
+        <v>0.58523501761644969</v>
       </c>
       <c r="I1">
-        <v>8</v>
+        <v>0.80806203282735078</v>
       </c>
       <c r="J1">
-        <v>9</v>
+        <v>0.53599520530876965</v>
       </c>
       <c r="K1">
-        <v>10</v>
+        <v>0.97509227948475474</v>
       </c>
       <c r="L1">
-        <v>11</v>
+        <v>0.35176386755202482</v>
       </c>
       <c r="M1">
-        <v>12</v>
+        <v>0.60849627157867181</v>
       </c>
       <c r="N1">
-        <v>13</v>
+        <v>0.88012193759774371</v>
       </c>
       <c r="O1">
-        <v>14</v>
+        <v>0.41404602837861404</v>
       </c>
       <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
+        <v>0.25238785045234902</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0.98278630377518839</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.98278630377518839</v>
+        <v>0.78253000344758028</v>
       </c>
       <c r="D2">
+        <v>4.5010958696151127E-3</v>
+      </c>
+      <c r="E2">
+        <v>0.40438864287881138</v>
+      </c>
+      <c r="F2">
+        <v>0.81137398915035008</v>
+      </c>
+      <c r="G2">
+        <v>0.94724838618038187</v>
+      </c>
+      <c r="H2">
+        <v>0.37522418078924524</v>
+      </c>
+      <c r="I2">
+        <v>0.82403262092859408</v>
+      </c>
+      <c r="J2">
+        <v>0.82450054338048928</v>
+      </c>
+      <c r="K2">
+        <v>0.16965860287232259</v>
+      </c>
+      <c r="L2">
+        <v>0.22462759831173384</v>
+      </c>
+      <c r="M2">
+        <v>0.79836528449204391</v>
+      </c>
+      <c r="N2">
+        <v>0.29218293409242757</v>
+      </c>
+      <c r="O2">
+        <v>0.22629865171434915</v>
+      </c>
+      <c r="P2">
+        <v>0.31887437573946054</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>0.50636093869825483</v>
       </c>
-      <c r="E2">
-        <v>0.73397479367659013</v>
-      </c>
-      <c r="F2">
-        <v>0.88924777405780919</v>
-      </c>
-      <c r="G2">
-        <v>0.69153678025465826</v>
-      </c>
-      <c r="H2">
-        <v>0.62990478407748318</v>
-      </c>
-      <c r="I2">
-        <v>0.58523501761644969</v>
-      </c>
-      <c r="J2">
-        <v>0.80806203282735078</v>
-      </c>
-      <c r="K2">
-        <v>0.53599520530876965</v>
-      </c>
-      <c r="L2">
-        <v>0.97509227948475474</v>
-      </c>
-      <c r="M2">
-        <v>0.35176386755202482</v>
-      </c>
-      <c r="N2">
-        <v>0.60849627157867181</v>
-      </c>
-      <c r="O2">
-        <v>0.88012193759774371</v>
-      </c>
-      <c r="P2">
-        <v>0.41404602837861404</v>
-      </c>
-      <c r="Q2">
-        <v>0.25238785045234902</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
       <c r="B3">
-        <v>0.98278630377518839</v>
+        <v>0.78253000344758028</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.78253000344758028</v>
+        <v>0.60284487256253583</v>
       </c>
       <c r="E3">
+        <v>0.17433611496492152</v>
+      </c>
+      <c r="F3">
+        <v>0.58158467286318194</v>
+      </c>
+      <c r="G3">
+        <v>0.57118261666852466</v>
+      </c>
+      <c r="H3">
+        <v>0.20000138842472759</v>
+      </c>
+      <c r="I3">
+        <v>0.37301285102265125</v>
+      </c>
+      <c r="J3">
+        <v>0.9575272197620196</v>
+      </c>
+      <c r="K3">
+        <v>0.32756947766755695</v>
+      </c>
+      <c r="L3">
+        <v>0.54160838933115285</v>
+      </c>
+      <c r="M3">
+        <v>0.57678125420974957</v>
+      </c>
+      <c r="N3">
+        <v>0.77077889635366204</v>
+      </c>
+      <c r="O3">
+        <v>0.70511804795708577</v>
+      </c>
+      <c r="P3">
+        <v>0.44130775090397045</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.73397479367659013</v>
+      </c>
+      <c r="B4">
         <v>4.5010958696151127E-3</v>
       </c>
-      <c r="F3">
-        <v>0.40438864287881138</v>
-      </c>
-      <c r="G3">
-        <v>0.81137398915035008</v>
-      </c>
-      <c r="H3">
-        <v>0.94724838618038187</v>
-      </c>
-      <c r="I3">
-        <v>0.37522418078924524</v>
-      </c>
-      <c r="J3">
-        <v>0.82403262092859408</v>
-      </c>
-      <c r="K3">
-        <v>0.82450054338048928</v>
-      </c>
-      <c r="L3">
-        <v>0.16965860287232259</v>
-      </c>
-      <c r="M3">
-        <v>0.22462759831173384</v>
-      </c>
-      <c r="N3">
-        <v>0.79836528449204391</v>
-      </c>
-      <c r="O3">
-        <v>0.29218293409242757</v>
-      </c>
-      <c r="P3">
-        <v>0.22629865171434915</v>
-      </c>
-      <c r="Q3">
-        <v>0.31887437573946054</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0.50636093869825483</v>
-      </c>
       <c r="C4">
-        <v>0.78253000344758028</v>
+        <v>0.60284487256253583</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.60284487256253583</v>
+        <v>0.58979174292751868</v>
       </c>
       <c r="F4">
+        <v>0.33330229879643547</v>
+      </c>
+      <c r="G4">
+        <v>0.34022932386634785</v>
+      </c>
+      <c r="H4">
+        <v>0.74665890957802217</v>
+      </c>
+      <c r="I4">
+        <v>0.32959003879860571</v>
+      </c>
+      <c r="J4">
+        <v>6.4081978820819674E-2</v>
+      </c>
+      <c r="K4">
+        <v>0.94243828176614275</v>
+      </c>
+      <c r="L4">
+        <v>0.34223389602429422</v>
+      </c>
+      <c r="M4">
+        <v>0.74244138860219644</v>
+      </c>
+      <c r="N4">
+        <v>0.67722644563183865</v>
+      </c>
+      <c r="O4">
+        <v>0.34587742968415758</v>
+      </c>
+      <c r="P4">
+        <v>0.94170982969026973</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.88924777405780919</v>
+      </c>
+      <c r="B5">
+        <v>0.40438864287881138</v>
+      </c>
+      <c r="C5">
         <v>0.17433611496492152</v>
       </c>
-      <c r="G4">
-        <v>0.58158467286318194</v>
-      </c>
-      <c r="H4">
-        <v>0.57118261666852466</v>
-      </c>
-      <c r="I4">
-        <v>0.20000138842472759</v>
-      </c>
-      <c r="J4">
-        <v>0.37301285102265125</v>
-      </c>
-      <c r="K4">
-        <v>0.9575272197620196</v>
-      </c>
-      <c r="L4">
-        <v>0.32756947766755695</v>
-      </c>
-      <c r="M4">
-        <v>0.54160838933115285</v>
-      </c>
-      <c r="N4">
-        <v>0.57678125420974957</v>
-      </c>
-      <c r="O4">
-        <v>0.77077889635366204</v>
-      </c>
-      <c r="P4">
-        <v>0.70511804795708577</v>
-      </c>
-      <c r="Q4">
-        <v>0.44130775090397045</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0.73397479367659013</v>
-      </c>
-      <c r="C5">
-        <v>4.5010958696151127E-3</v>
-      </c>
       <c r="D5">
-        <v>0.60284487256253583</v>
+        <v>0.58979174292751868</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.58979174292751868</v>
+        <v>0.99337376369869701</v>
       </c>
       <c r="G5">
+        <v>0.27960125734444374</v>
+      </c>
+      <c r="H5">
+        <v>0.39975845501629426</v>
+      </c>
+      <c r="I5">
+        <v>0.35404350947905616</v>
+      </c>
+      <c r="J5">
+        <v>0.71569113997257883</v>
+      </c>
+      <c r="K5">
+        <v>0.72885978719765732</v>
+      </c>
+      <c r="L5">
+        <v>0.70040814358129544</v>
+      </c>
+      <c r="M5">
+        <v>0.90907227159823023</v>
+      </c>
+      <c r="N5">
+        <v>0.21502694343680839</v>
+      </c>
+      <c r="O5">
+        <v>0.52745395160752651</v>
+      </c>
+      <c r="P5">
+        <v>0.21879078453976497</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.69153678025465826</v>
+      </c>
+      <c r="B6">
+        <v>0.81137398915035008</v>
+      </c>
+      <c r="C6">
+        <v>0.58158467286318194</v>
+      </c>
+      <c r="D6">
         <v>0.33330229879643547</v>
       </c>
-      <c r="H5">
-        <v>0.34022932386634785</v>
-      </c>
-      <c r="I5">
-        <v>0.74665890957802217</v>
-      </c>
-      <c r="J5">
-        <v>0.32959003879860571</v>
-      </c>
-      <c r="K5">
-        <v>6.4081978820819674E-2</v>
-      </c>
-      <c r="L5">
-        <v>0.94243828176614275</v>
-      </c>
-      <c r="M5">
-        <v>0.34223389602429422</v>
-      </c>
-      <c r="N5">
-        <v>0.74244138860219644</v>
-      </c>
-      <c r="O5">
-        <v>0.67722644563183865</v>
-      </c>
-      <c r="P5">
-        <v>0.34587742968415758</v>
-      </c>
-      <c r="Q5">
-        <v>0.94170982969026973</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0.88924777405780919</v>
-      </c>
-      <c r="C6">
-        <v>0.40438864287881138</v>
-      </c>
-      <c r="D6">
-        <v>0.17433611496492152</v>
-      </c>
       <c r="E6">
-        <v>0.58979174292751868</v>
+        <v>0.99337376369869701</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.99337376369869701</v>
+        <v>0.45640721876548596</v>
       </c>
       <c r="H6">
+        <v>0.82631240691370789</v>
+      </c>
+      <c r="I6">
+        <v>7.0361472433993932E-2</v>
+      </c>
+      <c r="J6">
+        <v>0.21161293376858592</v>
+      </c>
+      <c r="K6">
+        <v>0.15339902311551112</v>
+      </c>
+      <c r="L6">
+        <v>0.24932683514128684</v>
+      </c>
+      <c r="M6">
+        <v>0.49165127726986912</v>
+      </c>
+      <c r="N6">
+        <v>0.64016542464459625</v>
+      </c>
+      <c r="O6">
+        <v>0.40484411742044035</v>
+      </c>
+      <c r="P6">
+        <v>2.3788691069472123E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.62990478407748318</v>
+      </c>
+      <c r="B7">
+        <v>0.94724838618038187</v>
+      </c>
+      <c r="C7">
+        <v>0.57118261666852466</v>
+      </c>
+      <c r="D7">
+        <v>0.34022932386634785</v>
+      </c>
+      <c r="E7">
         <v>0.27960125734444374</v>
       </c>
-      <c r="I6">
-        <v>0.39975845501629426</v>
-      </c>
-      <c r="J6">
-        <v>0.35404350947905616</v>
-      </c>
-      <c r="K6">
-        <v>0.71569113997257883</v>
-      </c>
-      <c r="L6">
-        <v>0.72885978719765732</v>
-      </c>
-      <c r="M6">
-        <v>0.70040814358129544</v>
-      </c>
-      <c r="N6">
-        <v>0.90907227159823023</v>
-      </c>
-      <c r="O6">
-        <v>0.21502694343680839</v>
-      </c>
-      <c r="P6">
-        <v>0.52745395160752651</v>
-      </c>
-      <c r="Q6">
-        <v>0.21879078453976497</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0.69153678025465826</v>
-      </c>
-      <c r="C7">
-        <v>0.81137398915035008</v>
-      </c>
-      <c r="D7">
-        <v>0.58158467286318194</v>
-      </c>
-      <c r="E7">
-        <v>0.33330229879643547</v>
-      </c>
       <c r="F7">
-        <v>0.99337376369869701</v>
+        <v>0.45640721876548596</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.45640721876548596</v>
+        <v>0.18390650213337789</v>
       </c>
       <c r="I7">
+        <v>0.21909270671862235</v>
+      </c>
+      <c r="J7">
+        <v>0.22137962771514796</v>
+      </c>
+      <c r="K7">
+        <v>0.89640454614254894</v>
+      </c>
+      <c r="L7">
+        <v>0.29007254854697984</v>
+      </c>
+      <c r="M7">
+        <v>0.71664525748646091</v>
+      </c>
+      <c r="N7">
+        <v>0.44313987800930321</v>
+      </c>
+      <c r="O7">
+        <v>8.4703417433388273E-3</v>
+      </c>
+      <c r="P7">
+        <v>0.4948979071032702</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.58523501761644969</v>
+      </c>
+      <c r="B8">
+        <v>0.37522418078924524</v>
+      </c>
+      <c r="C8">
+        <v>0.20000138842472759</v>
+      </c>
+      <c r="D8">
+        <v>0.74665890957802217</v>
+      </c>
+      <c r="E8">
+        <v>0.39975845501629426</v>
+      </c>
+      <c r="F8">
         <v>0.82631240691370789</v>
       </c>
-      <c r="J7">
-        <v>7.0361472433993932E-2</v>
-      </c>
-      <c r="K7">
-        <v>0.21161293376858592</v>
-      </c>
-      <c r="L7">
-        <v>0.15339902311551112</v>
-      </c>
-      <c r="M7">
-        <v>0.24932683514128684</v>
-      </c>
-      <c r="N7">
-        <v>0.49165127726986912</v>
-      </c>
-      <c r="O7">
-        <v>0.64016542464459625</v>
-      </c>
-      <c r="P7">
-        <v>0.40484411742044035</v>
-      </c>
-      <c r="Q7">
-        <v>2.3788691069472123E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0.62990478407748318</v>
-      </c>
-      <c r="C8">
-        <v>0.94724838618038187</v>
-      </c>
-      <c r="D8">
-        <v>0.57118261666852466</v>
-      </c>
-      <c r="E8">
-        <v>0.34022932386634785</v>
-      </c>
-      <c r="F8">
-        <v>0.27960125734444374</v>
-      </c>
       <c r="G8">
-        <v>0.45640721876548596</v>
+        <v>0.18390650213337789</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.18390650213337789</v>
+        <v>0.99195159060445426</v>
       </c>
       <c r="J8">
+        <v>0.86809456119323414</v>
+      </c>
+      <c r="K8">
+        <v>0.23754321793640465</v>
+      </c>
+      <c r="L8">
+        <v>0.72356834311004659</v>
+      </c>
+      <c r="M8">
+        <v>2.2172095415460502E-2</v>
+      </c>
+      <c r="N8">
+        <v>0.21677922946762795</v>
+      </c>
+      <c r="O8">
+        <v>0.90138246781017484</v>
+      </c>
+      <c r="P8">
+        <v>0.53338151961624736</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.80806203282735078</v>
+      </c>
+      <c r="B9">
+        <v>0.82403262092859408</v>
+      </c>
+      <c r="C9">
+        <v>0.37301285102265125</v>
+      </c>
+      <c r="D9">
+        <v>0.32959003879860571</v>
+      </c>
+      <c r="E9">
+        <v>0.35404350947905616</v>
+      </c>
+      <c r="F9">
+        <v>7.0361472433993932E-2</v>
+      </c>
+      <c r="G9">
         <v>0.21909270671862235</v>
       </c>
-      <c r="K8">
-        <v>0.22137962771514796</v>
-      </c>
-      <c r="L8">
-        <v>0.89640454614254894</v>
-      </c>
-      <c r="M8">
-        <v>0.29007254854697984</v>
-      </c>
-      <c r="N8">
-        <v>0.71664525748646091</v>
-      </c>
-      <c r="O8">
-        <v>0.44313987800930321</v>
-      </c>
-      <c r="P8">
-        <v>8.4703417433388273E-3</v>
-      </c>
-      <c r="Q8">
-        <v>0.4948979071032702</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0.58523501761644969</v>
-      </c>
-      <c r="C9">
-        <v>0.37522418078924524</v>
-      </c>
-      <c r="D9">
-        <v>0.20000138842472759</v>
-      </c>
-      <c r="E9">
-        <v>0.74665890957802217</v>
-      </c>
-      <c r="F9">
-        <v>0.39975845501629426</v>
-      </c>
-      <c r="G9">
-        <v>0.82631240691370789</v>
-      </c>
       <c r="H9">
-        <v>0.18390650213337789</v>
+        <v>0.99195159060445426</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.99195159060445426</v>
+        <v>0.39616573899800145</v>
       </c>
       <c r="K9">
+        <v>0.78813726050913513</v>
+      </c>
+      <c r="L9">
+        <v>0.16137277219101565</v>
+      </c>
+      <c r="M9">
+        <v>0.72820594302703101</v>
+      </c>
+      <c r="N9">
+        <v>0.94100556584067807</v>
+      </c>
+      <c r="O9">
+        <v>0.3456929434399777</v>
+      </c>
+      <c r="P9">
+        <v>4.2667042136594113E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.53599520530876965</v>
+      </c>
+      <c r="B10">
+        <v>0.82450054338048928</v>
+      </c>
+      <c r="C10">
+        <v>0.9575272197620196</v>
+      </c>
+      <c r="D10">
+        <v>6.4081978820819674E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.71569113997257883</v>
+      </c>
+      <c r="F10">
+        <v>0.21161293376858592</v>
+      </c>
+      <c r="G10">
+        <v>0.22137962771514796</v>
+      </c>
+      <c r="H10">
         <v>0.86809456119323414</v>
       </c>
-      <c r="L9">
-        <v>0.23754321793640465</v>
-      </c>
-      <c r="M9">
-        <v>0.72356834311004659</v>
-      </c>
-      <c r="N9">
-        <v>2.2172095415460502E-2</v>
-      </c>
-      <c r="O9">
-        <v>0.21677922946762795</v>
-      </c>
-      <c r="P9">
-        <v>0.90138246781017484</v>
-      </c>
-      <c r="Q9">
-        <v>0.53338151961624736</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0.80806203282735078</v>
-      </c>
-      <c r="C10">
-        <v>0.82403262092859408</v>
-      </c>
-      <c r="D10">
-        <v>0.37301285102265125</v>
-      </c>
-      <c r="E10">
-        <v>0.32959003879860571</v>
-      </c>
-      <c r="F10">
-        <v>0.35404350947905616</v>
-      </c>
-      <c r="G10">
-        <v>7.0361472433993932E-2</v>
-      </c>
-      <c r="H10">
-        <v>0.21909270671862235</v>
-      </c>
       <c r="I10">
-        <v>0.99195159060445426</v>
+        <v>0.39616573899800145</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.39616573899800145</v>
+        <v>0.22852013706725405</v>
       </c>
       <c r="L10">
+        <v>0.45256965598969556</v>
+      </c>
+      <c r="M10">
+        <v>0.51246898889277914</v>
+      </c>
+      <c r="N10">
+        <v>0.8643354890278796</v>
+      </c>
+      <c r="O10">
+        <v>0.3031966189520795</v>
+      </c>
+      <c r="P10">
+        <v>0.39733489602185668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.97509227948475474</v>
+      </c>
+      <c r="B11">
+        <v>0.16965860287232259</v>
+      </c>
+      <c r="C11">
+        <v>0.32756947766755695</v>
+      </c>
+      <c r="D11">
+        <v>0.94243828176614275</v>
+      </c>
+      <c r="E11">
+        <v>0.72885978719765732</v>
+      </c>
+      <c r="F11">
+        <v>0.15339902311551112</v>
+      </c>
+      <c r="G11">
+        <v>0.89640454614254894</v>
+      </c>
+      <c r="H11">
+        <v>0.23754321793640465</v>
+      </c>
+      <c r="I11">
         <v>0.78813726050913513</v>
       </c>
-      <c r="M10">
-        <v>0.16137277219101565</v>
-      </c>
-      <c r="N10">
-        <v>0.72820594302703101</v>
-      </c>
-      <c r="O10">
-        <v>0.94100556584067807</v>
-      </c>
-      <c r="P10">
-        <v>0.3456929434399777</v>
-      </c>
-      <c r="Q10">
-        <v>4.2667042136594113E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>0.53599520530876965</v>
-      </c>
-      <c r="C11">
-        <v>0.82450054338048928</v>
-      </c>
-      <c r="D11">
-        <v>0.9575272197620196</v>
-      </c>
-      <c r="E11">
-        <v>6.4081978820819674E-2</v>
-      </c>
-      <c r="F11">
-        <v>0.71569113997257883</v>
-      </c>
-      <c r="G11">
-        <v>0.21161293376858592</v>
-      </c>
-      <c r="H11">
-        <v>0.22137962771514796</v>
-      </c>
-      <c r="I11">
-        <v>0.86809456119323414</v>
-      </c>
       <c r="J11">
-        <v>0.39616573899800145</v>
+        <v>0.22852013706725405</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.22852013706725405</v>
+        <v>0.4483559984872707</v>
       </c>
       <c r="M11">
+        <v>0.62815454008410521</v>
+      </c>
+      <c r="N11">
+        <v>0.41962617716668194</v>
+      </c>
+      <c r="O11">
+        <v>0.35895665834564894</v>
+      </c>
+      <c r="P11">
+        <v>0.51946314187411646</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.35176386755202482</v>
+      </c>
+      <c r="B12">
+        <v>0.22462759831173384</v>
+      </c>
+      <c r="C12">
+        <v>0.54160838933115285</v>
+      </c>
+      <c r="D12">
+        <v>0.34223389602429422</v>
+      </c>
+      <c r="E12">
+        <v>0.70040814358129544</v>
+      </c>
+      <c r="F12">
+        <v>0.24932683514128684</v>
+      </c>
+      <c r="G12">
+        <v>0.29007254854697984</v>
+      </c>
+      <c r="H12">
+        <v>0.72356834311004659</v>
+      </c>
+      <c r="I12">
+        <v>0.16137277219101565</v>
+      </c>
+      <c r="J12">
         <v>0.45256965598969556</v>
       </c>
-      <c r="N11">
-        <v>0.51246898889277914</v>
-      </c>
-      <c r="O11">
-        <v>0.8643354890278796</v>
-      </c>
-      <c r="P11">
-        <v>0.3031966189520795</v>
-      </c>
-      <c r="Q11">
-        <v>0.39733489602185668</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>0.97509227948475474</v>
-      </c>
-      <c r="C12">
-        <v>0.16965860287232259</v>
-      </c>
-      <c r="D12">
-        <v>0.32756947766755695</v>
-      </c>
-      <c r="E12">
-        <v>0.94243828176614275</v>
-      </c>
-      <c r="F12">
-        <v>0.72885978719765732</v>
-      </c>
-      <c r="G12">
-        <v>0.15339902311551112</v>
-      </c>
-      <c r="H12">
-        <v>0.89640454614254894</v>
-      </c>
-      <c r="I12">
-        <v>0.23754321793640465</v>
-      </c>
-      <c r="J12">
-        <v>0.78813726050913513</v>
-      </c>
       <c r="K12">
-        <v>0.22852013706725405</v>
+        <v>0.4483559984872707</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0.4483559984872707</v>
+        <v>0.85438476941927122</v>
       </c>
       <c r="N12">
+        <v>0.5927891136322393</v>
+      </c>
+      <c r="O12">
+        <v>0.8711092634898977</v>
+      </c>
+      <c r="P12">
+        <v>0.62673802986720006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.60849627157867181</v>
+      </c>
+      <c r="B13">
+        <v>0.79836528449204391</v>
+      </c>
+      <c r="C13">
+        <v>0.57678125420974957</v>
+      </c>
+      <c r="D13">
+        <v>0.74244138860219644</v>
+      </c>
+      <c r="E13">
+        <v>0.90907227159823023</v>
+      </c>
+      <c r="F13">
+        <v>0.49165127726986912</v>
+      </c>
+      <c r="G13">
+        <v>0.71664525748646091</v>
+      </c>
+      <c r="H13">
+        <v>2.2172095415460502E-2</v>
+      </c>
+      <c r="I13">
+        <v>0.72820594302703101</v>
+      </c>
+      <c r="J13">
+        <v>0.51246898889277914</v>
+      </c>
+      <c r="K13">
         <v>0.62815454008410521</v>
       </c>
-      <c r="O12">
-        <v>0.41962617716668194</v>
-      </c>
-      <c r="P12">
-        <v>0.35895665834564894</v>
-      </c>
-      <c r="Q12">
-        <v>0.51946314187411646</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>0.35176386755202482</v>
-      </c>
-      <c r="C13">
-        <v>0.22462759831173384</v>
-      </c>
-      <c r="D13">
-        <v>0.54160838933115285</v>
-      </c>
-      <c r="E13">
-        <v>0.34223389602429422</v>
-      </c>
-      <c r="F13">
-        <v>0.70040814358129544</v>
-      </c>
-      <c r="G13">
-        <v>0.24932683514128684</v>
-      </c>
-      <c r="H13">
-        <v>0.29007254854697984</v>
-      </c>
-      <c r="I13">
-        <v>0.72356834311004659</v>
-      </c>
-      <c r="J13">
-        <v>0.16137277219101565</v>
-      </c>
-      <c r="K13">
-        <v>0.45256965598969556</v>
-      </c>
       <c r="L13">
-        <v>0.4483559984872707</v>
+        <v>0.85438476941927122</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>0.85438476941927122</v>
+        <v>0.58056027074821481</v>
       </c>
       <c r="O13">
+        <v>0.7109082374162673</v>
+      </c>
+      <c r="P13">
+        <v>0.22010845846766691</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.88012193759774371</v>
+      </c>
+      <c r="B14">
+        <v>0.29218293409242757</v>
+      </c>
+      <c r="C14">
+        <v>0.77077889635366204</v>
+      </c>
+      <c r="D14">
+        <v>0.67722644563183865</v>
+      </c>
+      <c r="E14">
+        <v>0.21502694343680839</v>
+      </c>
+      <c r="F14">
+        <v>0.64016542464459625</v>
+      </c>
+      <c r="G14">
+        <v>0.44313987800930321</v>
+      </c>
+      <c r="H14">
+        <v>0.21677922946762795</v>
+      </c>
+      <c r="I14">
+        <v>0.94100556584067807</v>
+      </c>
+      <c r="J14">
+        <v>0.8643354890278796</v>
+      </c>
+      <c r="K14">
+        <v>0.41962617716668194</v>
+      </c>
+      <c r="L14">
         <v>0.5927891136322393</v>
       </c>
-      <c r="P13">
-        <v>0.8711092634898977</v>
-      </c>
-      <c r="Q13">
-        <v>0.62673802986720006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0.60849627157867181</v>
-      </c>
-      <c r="C14">
-        <v>0.79836528449204391</v>
-      </c>
-      <c r="D14">
-        <v>0.57678125420974957</v>
-      </c>
-      <c r="E14">
-        <v>0.74244138860219644</v>
-      </c>
-      <c r="F14">
-        <v>0.90907227159823023</v>
-      </c>
-      <c r="G14">
-        <v>0.49165127726986912</v>
-      </c>
-      <c r="H14">
-        <v>0.71664525748646091</v>
-      </c>
-      <c r="I14">
-        <v>2.2172095415460502E-2</v>
-      </c>
-      <c r="J14">
-        <v>0.72820594302703101</v>
-      </c>
-      <c r="K14">
-        <v>0.51246898889277914</v>
-      </c>
-      <c r="L14">
-        <v>0.62815454008410521</v>
-      </c>
       <c r="M14">
-        <v>0.85438476941927122</v>
+        <v>0.58056027074821481</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14">
-        <v>0.58056027074821481</v>
+        <v>0.18983648577319812</v>
       </c>
       <c r="P14">
+        <v>0.14417540640168669</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.41404602837861404</v>
+      </c>
+      <c r="B15">
+        <v>0.22629865171434915</v>
+      </c>
+      <c r="C15">
+        <v>0.70511804795708577</v>
+      </c>
+      <c r="D15">
+        <v>0.34587742968415758</v>
+      </c>
+      <c r="E15">
+        <v>0.52745395160752651</v>
+      </c>
+      <c r="F15">
+        <v>0.40484411742044035</v>
+      </c>
+      <c r="G15">
+        <v>8.4703417433388273E-3</v>
+      </c>
+      <c r="H15">
+        <v>0.90138246781017484</v>
+      </c>
+      <c r="I15">
+        <v>0.3456929434399777</v>
+      </c>
+      <c r="J15">
+        <v>0.3031966189520795</v>
+      </c>
+      <c r="K15">
+        <v>0.35895665834564894</v>
+      </c>
+      <c r="L15">
+        <v>0.8711092634898977</v>
+      </c>
+      <c r="M15">
         <v>0.7109082374162673</v>
       </c>
-      <c r="Q14">
-        <v>0.22010845846766691</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0.88012193759774371</v>
-      </c>
-      <c r="C15">
-        <v>0.29218293409242757</v>
-      </c>
-      <c r="D15">
-        <v>0.77077889635366204</v>
-      </c>
-      <c r="E15">
-        <v>0.67722644563183865</v>
-      </c>
-      <c r="F15">
-        <v>0.21502694343680839</v>
-      </c>
-      <c r="G15">
-        <v>0.64016542464459625</v>
-      </c>
-      <c r="H15">
-        <v>0.44313987800930321</v>
-      </c>
-      <c r="I15">
-        <v>0.21677922946762795</v>
-      </c>
-      <c r="J15">
-        <v>0.94100556584067807</v>
-      </c>
-      <c r="K15">
-        <v>0.8643354890278796</v>
-      </c>
-      <c r="L15">
-        <v>0.41962617716668194</v>
-      </c>
-      <c r="M15">
-        <v>0.5927891136322393</v>
-      </c>
       <c r="N15">
-        <v>0.58056027074821481</v>
+        <v>0.18983648577319812</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
       <c r="P15">
-        <v>0.18983648577319812</v>
-      </c>
-      <c r="Q15">
+        <v>0.38692769695651974</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.25238785045234902</v>
+      </c>
+      <c r="B16">
+        <v>0.31887437573946054</v>
+      </c>
+      <c r="C16">
+        <v>0.44130775090397045</v>
+      </c>
+      <c r="D16">
+        <v>0.94170982969026973</v>
+      </c>
+      <c r="E16">
+        <v>0.21879078453976497</v>
+      </c>
+      <c r="F16">
+        <v>2.3788691069472123E-2</v>
+      </c>
+      <c r="G16">
+        <v>0.4948979071032702</v>
+      </c>
+      <c r="H16">
+        <v>0.53338151961624736</v>
+      </c>
+      <c r="I16">
+        <v>4.2667042136594113E-2</v>
+      </c>
+      <c r="J16">
+        <v>0.39733489602185668</v>
+      </c>
+      <c r="K16">
+        <v>0.51946314187411646</v>
+      </c>
+      <c r="L16">
+        <v>0.62673802986720006</v>
+      </c>
+      <c r="M16">
+        <v>0.22010845846766691</v>
+      </c>
+      <c r="N16">
         <v>0.14417540640168669</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>0.41404602837861404</v>
-      </c>
-      <c r="C16">
-        <v>0.22629865171434915</v>
-      </c>
-      <c r="D16">
-        <v>0.70511804795708577</v>
-      </c>
-      <c r="E16">
-        <v>0.34587742968415758</v>
-      </c>
-      <c r="F16">
-        <v>0.52745395160752651</v>
-      </c>
-      <c r="G16">
-        <v>0.40484411742044035</v>
-      </c>
-      <c r="H16">
-        <v>8.4703417433388273E-3</v>
-      </c>
-      <c r="I16">
-        <v>0.90138246781017484</v>
-      </c>
-      <c r="J16">
-        <v>0.3456929434399777</v>
-      </c>
-      <c r="K16">
-        <v>0.3031966189520795</v>
-      </c>
-      <c r="L16">
-        <v>0.35895665834564894</v>
-      </c>
-      <c r="M16">
-        <v>0.8711092634898977</v>
-      </c>
-      <c r="N16">
-        <v>0.7109082374162673</v>
-      </c>
       <c r="O16">
-        <v>0.18983648577319812</v>
+        <v>0.38692769695651974</v>
       </c>
       <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>0.38692769695651974</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>0.25238785045234902</v>
-      </c>
-      <c r="C17">
-        <v>0.31887437573946054</v>
-      </c>
-      <c r="D17">
-        <v>0.44130775090397045</v>
-      </c>
-      <c r="E17">
-        <v>0.94170982969026973</v>
-      </c>
-      <c r="F17">
-        <v>0.21879078453976497</v>
-      </c>
-      <c r="G17">
-        <v>2.3788691069472123E-2</v>
-      </c>
-      <c r="H17">
-        <v>0.4948979071032702</v>
-      </c>
-      <c r="I17">
-        <v>0.53338151961624736</v>
-      </c>
-      <c r="J17">
-        <v>4.2667042136594113E-2</v>
-      </c>
-      <c r="K17">
-        <v>0.39733489602185668</v>
-      </c>
-      <c r="L17">
-        <v>0.51946314187411646</v>
-      </c>
-      <c r="M17">
-        <v>0.62673802986720006</v>
-      </c>
-      <c r="N17">
-        <v>0.22010845846766691</v>
-      </c>
-      <c r="O17">
-        <v>0.14417540640168669</v>
-      </c>
-      <c r="P17">
-        <v>0.38692769695651974</v>
-      </c>
-      <c r="Q17">
         <v>1</v>
       </c>
     </row>
@@ -4132,15 +4134,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4428,6 +4421,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4449,14 +4451,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A33AA7F4-51CC-46CE-816E-9CAB67B26DBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F291531A-8552-416A-951C-C6D10D48BDBD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4477,6 +4471,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A33AA7F4-51CC-46CE-816E-9CAB67B26DBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89BFA361-931E-4B88-854C-2477F4226589}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
do not touch; fragile
</commit_message>
<xml_diff>
--- a/visualization_wip.xlsx
+++ b/visualization_wip.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E95F18-B512-4889-851B-ECFE31001B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C683CA0-E963-4F56-A965-62B9A334A8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="533" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="Overtime_hrs">SUM('[1]YEARLY TIMESHEET'!$I$11+'[1]YEARLY TIMESHEET'!$I$22+'[1]YEARLY TIMESHEET'!$I$33+'[1]YEARLY TIMESHEET'!$I$44)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Tournament!$A$1:$K$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Tournament!$A$2:$K$19</definedName>
     <definedName name="RegularHrs">SUM('[1]YEARLY TIMESHEET'!$F$11+'[1]YEARLY TIMESHEET'!$F$22+'[1]YEARLY TIMESHEET'!$F$33+'[1]YEARLY TIMESHEET'!$F$44)</definedName>
     <definedName name="Total_Overtime_hrs">SUM('[2]YEARLY TIMESHEET'!$I$12,'[2]YEARLY TIMESHEET'!$I$23,'[2]YEARLY TIMESHEET'!$I$34,'[2]YEARLY TIMESHEET'!$I$46,'[2]YEARLY TIMESHEET'!$I$57,'[2]YEARLY TIMESHEET'!$I$68,'[2]YEARLY TIMESHEET'!$I$80,'[2]YEARLY TIMESHEET'!$I$91,'[2]YEARLY TIMESHEET'!$I$102,'[2]YEARLY TIMESHEET'!$I$114,'[2]YEARLY TIMESHEET'!$I$125,'[2]YEARLY TIMESHEET'!$I$136)</definedName>
     <definedName name="Total_Regular_hrs">SUM('[2]YEARLY TIMESHEET'!$G$12,'[2]YEARLY TIMESHEET'!$G$23,'[2]YEARLY TIMESHEET'!$G$34,'[2]YEARLY TIMESHEET'!$G$46,'[2]YEARLY TIMESHEET'!$G$57,'[2]YEARLY TIMESHEET'!$G$68,'[2]YEARLY TIMESHEET'!$G$80,'[2]YEARLY TIMESHEET'!$G$91,'[2]YEARLY TIMESHEET'!$G$102,'[2]YEARLY TIMESHEET'!$G$114,'[2]YEARLY TIMESHEET'!$G$125,'[2]YEARLY TIMESHEET'!$G$136)</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="5">
   <si>
     <t>ABOUT THIS TEMPLATE</t>
   </si>
@@ -50,12 +50,18 @@
   <si>
     <t>Fill in the teams that are playing, and as winners are determined, complete the bracket until the champion is crowned.</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,13 +85,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="24"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1" tint="0.14996795556505021"/>
       <name val="Calibri"/>
@@ -99,6 +98,20 @@
       <name val="Cambria"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -185,14 +198,14 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -200,9 +213,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -214,12 +224,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="2">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="2">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2 2" xfId="2" xr:uid="{816C1F22-910F-4B91-A00B-7D31A264BF92}"/>
@@ -313,13 +329,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1071</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>214245</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2524</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>214245</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -340,8 +356,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2112900" y="214245"/>
-          <a:ext cx="1220653" cy="1001486"/>
+          <a:off x="2119431" y="717165"/>
+          <a:ext cx="1220653" cy="1005840"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="67" cy="204"/>
         </a:xfrm>
@@ -474,13 +490,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2079170</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>245370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1219199</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>231954</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -501,8 +517,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5410199" y="746113"/>
-          <a:ext cx="1262743" cy="1989555"/>
+          <a:off x="5416730" y="1251210"/>
+          <a:ext cx="1258389" cy="1998264"/>
           <a:chOff x="460" y="254"/>
           <a:chExt cx="69" cy="408"/>
         </a:xfrm>
@@ -635,13 +651,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>977900</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>495300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>977900</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -692,13 +708,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1006162</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>241479</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>241479</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -749,13 +765,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>977900</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>977900</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -806,13 +822,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>825500</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>15875</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -833,8 +849,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10896600" y="2002971"/>
-          <a:ext cx="825500" cy="4021818"/>
+          <a:off x="10911840" y="2514600"/>
+          <a:ext cx="825500" cy="4039235"/>
           <a:chOff x="655" y="467"/>
           <a:chExt cx="42" cy="848"/>
         </a:xfrm>
@@ -963,13 +979,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>256236</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>256236</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -990,8 +1006,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2111829" y="2259207"/>
-          <a:ext cx="1228726" cy="1001486"/>
+          <a:off x="2118360" y="2770836"/>
+          <a:ext cx="1228726" cy="1005840"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="65" cy="204"/>
         </a:xfrm>
@@ -1124,13 +1140,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>252346</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>252346</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1151,8 +1167,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2121354" y="4258289"/>
-          <a:ext cx="1209675" cy="1502228"/>
+          <a:off x="2127885" y="5257800"/>
+          <a:ext cx="1209675" cy="1029586"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="62" cy="204"/>
         </a:xfrm>
@@ -1254,7 +1270,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="364" y="284"/>
+            <a:off x="364" y="263"/>
             <a:ext cx="31" cy="0"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -1285,13 +1301,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>269651</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>13678</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>269651</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1312,8 +1328,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2121353" y="6779308"/>
-          <a:ext cx="1223354" cy="1001486"/>
+          <a:off x="2127884" y="7310531"/>
+          <a:ext cx="1223354" cy="1005840"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="64" cy="204"/>
         </a:xfrm>
@@ -1445,14 +1461,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>8292</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>296482</xdr:rowOff>
+      <xdr:colOff>8291</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>23209</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:colOff>23208</xdr:colOff>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>296482</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1473,8 +1489,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="16347749" y="4302425"/>
-          <a:ext cx="1223231" cy="1502228"/>
+          <a:off x="16376051" y="5257800"/>
+          <a:ext cx="1218877" cy="1073722"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="64" cy="204"/>
         </a:xfrm>
@@ -1576,7 +1592,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm flipV="1">
-            <a:off x="365" y="262"/>
+            <a:off x="365" y="256"/>
             <a:ext cx="32" cy="0"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -1607,13 +1623,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>13415</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>269652</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>9793</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>269652</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1634,8 +1650,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="16352872" y="6779309"/>
-          <a:ext cx="1204692" cy="1001486"/>
+          <a:off x="16381175" y="7310532"/>
+          <a:ext cx="1200338" cy="1005840"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="63" cy="204"/>
         </a:xfrm>
@@ -1768,13 +1784,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>993</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>256236</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>4</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>256236</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1795,8 +1811,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16340450" y="256236"/>
-          <a:ext cx="1207325" cy="1001486"/>
+          <a:off x="16368753" y="759156"/>
+          <a:ext cx="1202971" cy="1005840"/>
           <a:chOff x="861" y="153"/>
           <a:chExt cx="60" cy="204"/>
         </a:xfrm>
@@ -1929,13 +1945,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>12695</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>269651</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1152241</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>269651</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1956,8 +1972,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16352152" y="2272622"/>
-          <a:ext cx="1139546" cy="1001486"/>
+          <a:off x="16380455" y="2784251"/>
+          <a:ext cx="1139546" cy="1005840"/>
           <a:chOff x="856" y="153"/>
           <a:chExt cx="65" cy="204"/>
         </a:xfrm>
@@ -2090,13 +2106,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>257175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>23204</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>257175</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2117,8 +2133,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5472793" y="5264604"/>
-          <a:ext cx="1223354" cy="2002971"/>
+          <a:off x="5474970" y="5789295"/>
+          <a:ext cx="1223354" cy="2011680"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="64" cy="204"/>
         </a:xfrm>
@@ -2251,13 +2267,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>276225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1170586</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>257175</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2278,8 +2294,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13008429" y="776968"/>
-          <a:ext cx="1170586" cy="1983921"/>
+          <a:off x="13030200" y="1282065"/>
+          <a:ext cx="1170586" cy="1992630"/>
           <a:chOff x="861" y="153"/>
           <a:chExt cx="60" cy="204"/>
         </a:xfrm>
@@ -2412,13 +2428,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>276225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1170586</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>257175</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2439,8 +2455,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13008429" y="5283654"/>
-          <a:ext cx="1170586" cy="1983921"/>
+          <a:off x="13030200" y="5808345"/>
+          <a:ext cx="1170586" cy="1992630"/>
           <a:chOff x="861" y="153"/>
           <a:chExt cx="60" cy="204"/>
         </a:xfrm>
@@ -3059,24 +3075,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="82.109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="2.77734375" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.77734375" style="9"/>
+    <col min="1" max="1" width="2.77734375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="82.109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="2.77734375" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="8.77734375" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3092,10 +3108,10 @@
     <tabColor indexed="40"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.88671875" defaultRowHeight="39.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3112,202 +3128,885 @@
     <col min="12" max="16384" width="16.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="4">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="str">
+        <f ca="1">IF(A19=TRUE,'Win probabilities'!A5,"")</f>
+        <v/>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="10" t="str">
+        <f ca="1">IF(H19=TRUE,'Win probabilities'!I13,"")</f>
+        <v/>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="b">
-        <f ca="1">AND(C2=1,C6=3)</f>
+      <c r="B2" s="11" t="b">
+        <f ca="1">AND(C3=1,C7=3)</f>
         <v>1</v>
       </c>
-      <c r="D1" s="3">
-        <f ca="1">IF(C1=TRUE,'Win probabilities'!A3)</f>
+      <c r="C2" s="3">
+        <f ca="1">IF(B2=TRUE,'Win probabilities'!A3," ")</f>
         <v>0.50636093869825483</v>
       </c>
-      <c r="K1" s="4">
+      <c r="E2" s="10" t="str">
+        <f ca="1">IF(B19=TRUE,'Win probabilities'!A6,"")</f>
+        <v/>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="10" t="str">
+        <f ca="1">IF(I19=TRUE,'Win probabilities'!I14,"")</f>
+        <v/>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f ca="1">IF(J2=TRUE,'Win probabilities'!I11," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J2" s="11" t="b">
+        <f ca="1">AND(I3=9,I7=11)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="3">
+      <c r="L2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="3">
         <f>'Win probabilities'!A2</f>
         <v>0.98278630377518839</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6">
-        <f ca="1">IF(RAND()&lt;A2,A1,A3)</f>
+      <c r="B3" s="11"/>
+      <c r="C3" s="5">
+        <f ca="1">IF(RAND()&lt;A3,A2,A4)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="4">
+      <c r="E3" s="10">
+        <f ca="1">IF(C19=TRUE,'Win probabilities'!A7,"")</f>
+        <v>0.62990478407748318</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="10" t="str">
+        <f ca="1">IF(J19=TRUE,'Win probabilities'!I15,"")</f>
+        <v/>
+      </c>
+      <c r="I3" s="5">
+        <f ca="1">IF(RAND()&lt;K3,K2,K4)</f>
+        <v>10</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="3">
+        <f>'Win probabilities'!I10</f>
+        <v>0.39616573899800145</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="b">
-        <f ca="1">AND(C2=2,C6=3)</f>
+      <c r="B4" s="11" t="b">
+        <f ca="1">AND(C3=2,C7=3)</f>
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="b">
-        <f ca="1">IF(C3=TRUE,'Win probabilities'!B3)</f>
+      <c r="C4" s="3" t="str">
+        <f ca="1">IF(B4=TRUE,'Win probabilities'!B3," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f ca="1">IF(D19=TRUE,'Win probabilities'!A8,"")</f>
+        <v/>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f ca="1">IF(K19=TRUE,'Win probabilities'!I16,"")</f>
+        <v/>
+      </c>
+      <c r="I4" s="3" t="str">
+        <f ca="1">IF(J4=TRUE,'Win probabilities'!J11," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J4" s="11" t="b">
+        <f ca="1">AND(I3=10,I7=11)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K4" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="E4" s="7">
-        <f ca="1">IF(RAND()&lt;SUM(D1:D7),C2,C6)</f>
+      <c r="L4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="11"/>
+      <c r="E5" s="6">
+        <f ca="1">IF(RAND()&lt;SUM(C2,C4,C6,C8),C3,C7)</f>
         <v>1</v>
       </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="b">
-        <f ca="1">AND(C2=1,C6=4)</f>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6">
+        <f ca="1">IF(RAND()&lt;SUM(I2,I4,I6,I8),I3,I7)</f>
+        <v>10</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="L5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11" t="b">
+        <f ca="1">AND(C3=1,C7=4)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="3" t="b">
-        <f ca="1">IF(C5=TRUE,'Win probabilities'!A4)</f>
+      <c r="C6" s="3" t="str">
+        <f ca="1">IF(B6=TRUE,'Win probabilities'!A4," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E6" s="10" t="str">
+        <f ca="1">IF(A20=TRUE,'Win probabilities'!B5,"")</f>
+        <v/>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="10">
+        <f ca="1">IF(H20=TRUE,'Win probabilities'!J13,"")</f>
+        <v>0.51246898889277914</v>
+      </c>
+      <c r="I6" s="3" t="str">
+        <f ca="1">IF(J6=TRUE,'Win probabilities'!I12," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J6" s="11" t="b">
+        <f ca="1">AND(I3=9,I7=12)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K6" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="3">
+      <c r="L6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="3">
         <f>'Win probabilities'!C4</f>
         <v>0.60284487256253583</v>
       </c>
-      <c r="C6" s="6">
-        <f ca="1">IF(RAND()&lt;A6,A5,A7)</f>
-        <v>3</v>
-      </c>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A7" s="4">
+      <c r="B7" s="11"/>
+      <c r="C7" s="5">
+        <f ca="1">IF(RAND()&lt;A7,A6,A8)</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="10" t="str">
+        <f ca="1">IF(B20=TRUE,'Win probabilities'!B6,"")</f>
+        <v/>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="10" t="str">
+        <f ca="1">IF(I20=TRUE,'Win probabilities'!J14,"")</f>
+        <v/>
+      </c>
+      <c r="I7" s="5">
+        <f ca="1">IF(RAND()&lt;K7,K6,K8)</f>
+        <v>12</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="3">
+        <f>'Win probabilities'!K12</f>
+        <v>0.4483559984872707</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="b">
-        <f ca="1">AND(C2=2,C6=4)</f>
+      <c r="B8" s="11" t="b">
+        <f ca="1">AND(C3=2,C7=4)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="3" t="b">
-        <f ca="1">IF(C7=TRUE,'Win probabilities'!B4)</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
+      <c r="C8" s="3" t="str">
+        <f ca="1">IF(B8=TRUE,'Win probabilities'!B4," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E8" s="10" t="str">
+        <f ca="1">IF(C20=TRUE,'Win probabilities'!B7,"")</f>
+        <v/>
+      </c>
+      <c r="G8" s="10" t="str">
+        <f ca="1">IF(J20=TRUE,'Win probabilities'!J15,"")</f>
+        <v/>
+      </c>
+      <c r="I8" s="3">
+        <f ca="1">IF(J8=TRUE,'Win probabilities'!J12," ")</f>
+        <v>0.45256965598969556</v>
+      </c>
+      <c r="J8" s="11" t="b">
+        <f ca="1">AND(I3=10,I7=12)</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A9" s="4">
+      <c r="L8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B9" s="11"/>
+      <c r="E9" s="10" t="str">
+        <f ca="1">IF(D20=TRUE,'Win probabilities'!B8,"")</f>
+        <v/>
+      </c>
+      <c r="F9" s="7">
+        <f ca="1">IF(RAND()&lt;SUM(E1:E4,E6:E13,E15:E18),E5,E14)</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="10" t="str">
+        <f ca="1">IF(K20=TRUE,'Win probabilities'!J16,"")</f>
+        <v/>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="N9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B10" s="11"/>
+      <c r="E10" s="10" t="str">
+        <f ca="1">IF(A21=TRUE,'Win probabilities'!C5,"")</f>
+        <v/>
+      </c>
+      <c r="G10" s="10" t="str">
+        <f ca="1">IF(H21=TRUE,'Win probabilities'!K13,"")</f>
+        <v/>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="N10" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="3" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A11" s="4">
         <v>5</v>
       </c>
-      <c r="K9" s="4">
+      <c r="B11" s="11" t="b">
+        <f ca="1">AND(C12=5,C16=7)</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <f ca="1">IF(B11=TRUE,'Win probabilities'!E7," ")</f>
+        <v>0.27960125734444374</v>
+      </c>
+      <c r="E11" s="10" t="str">
+        <f ca="1">IF(B21=TRUE,'Win probabilities'!C6,"")</f>
+        <v/>
+      </c>
+      <c r="F11" s="7">
+        <f ca="1">IF(RAND()&lt;SUM(G1:G4,G6:G13,G15:G18),G5,G14)</f>
+        <v>10</v>
+      </c>
+      <c r="G11" s="10" t="str">
+        <f ca="1">IF(I21=TRUE,'Win probabilities'!K14,"")</f>
+        <v/>
+      </c>
+      <c r="I11" s="3">
+        <f ca="1">IF(J11=TRUE,'Win probabilities'!M15," ")</f>
+        <v>0.7109082374162673</v>
+      </c>
+      <c r="J11" s="11" t="b">
+        <f ca="1">AND(I12=13,I16=15)</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A10" s="3">
+      <c r="N11" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="3">
         <f>'Win probabilities'!E6</f>
         <v>0.99337376369869701</v>
       </c>
-      <c r="C10" s="3" t="b">
-        <f ca="1">AND(C11=5,C15=7)</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <f ca="1">IF(C10=TRUE,'Win probabilities'!E7)</f>
-        <v>0.27960125734444374</v>
-      </c>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="C11" s="6">
-        <f ca="1">IF(RAND()&lt;A10,A9,A12)</f>
+      <c r="B12" s="11"/>
+      <c r="C12" s="5">
+        <f ca="1">IF(RAND()&lt;A12,A11,A13)</f>
         <v>5</v>
       </c>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="4">
+      <c r="E12" s="10" t="str">
+        <f ca="1">IF(C21=TRUE,'Win probabilities'!C7,"")</f>
+        <v/>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="10" t="str">
+        <f ca="1">IF(J21=TRUE,'Win probabilities'!K15,"")</f>
+        <v/>
+      </c>
+      <c r="I12" s="5">
+        <f ca="1">IF(RAND()&lt;K12,K11,K13)</f>
+        <v>13</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="3">
+        <f>'Win probabilities'!M14</f>
+        <v>0.58056027074821481</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A13" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="3" t="b">
-        <f ca="1">AND(C11=6,C15=7)</f>
+      <c r="B13" s="11" t="b">
+        <f ca="1">AND(C12=6,C16=7)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="3" t="b">
-        <f ca="1">IF(C12=TRUE,'Win probabilities'!F7)</f>
+      <c r="C13" s="3" t="str">
+        <f ca="1">IF(B13=TRUE,'Win probabilities'!F7," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E13" s="10" t="str">
+        <f ca="1">IF(D21=TRUE,'Win probabilities'!C8,"")</f>
+        <v/>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="10" t="str">
+        <f ca="1">IF(K21=TRUE,'Win probabilities'!K16,"")</f>
+        <v/>
+      </c>
+      <c r="I13" s="3" t="str">
+        <f ca="1">IF(J13=TRUE,'Win probabilities'!N15," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J13" s="11" t="b">
+        <f ca="1">AND(I12=14,I16=15)</f>
         <v>0</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K13" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="E13" s="7">
-        <f ca="1">IF(RAND()&lt;SUM(D10:D16),C11,C15)</f>
+      <c r="N13" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B14" s="11"/>
+      <c r="E14" s="6">
+        <f ca="1">IF(RAND()&lt;SUM(C11,C13,C15,C17),C12,C16)</f>
         <v>7</v>
       </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="4">
+      <c r="F14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="6">
+        <f ca="1">IF(RAND()&lt;SUM(I11,I13,I15,I17),I12,I16)</f>
+        <v>13</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="N14" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A15" s="4">
         <v>7</v>
       </c>
-      <c r="C14" s="3" t="b">
-        <f ca="1">AND(C11=5,C15=8)</f>
+      <c r="B15" s="11" t="b">
+        <f ca="1">AND(C12=5,C16=8)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="3" t="b">
-        <f ca="1">IF(C14=TRUE,'Win probabilities'!E8)</f>
+      <c r="C15" s="3" t="str">
+        <f ca="1">IF(B15=TRUE,'Win probabilities'!E8," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E15" s="10" t="str">
+        <f ca="1">IF(A22=TRUE,'Win probabilities'!D5,"")</f>
+        <v/>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="10" t="str">
+        <f ca="1">IF(H22=TRUE,'Win probabilities'!L13,"")</f>
+        <v/>
+      </c>
+      <c r="I15" s="3" t="str">
+        <f ca="1">IF(J15=TRUE,'Win probabilities'!M16," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J15" s="11" t="b">
+        <f ca="1">AND(I12=13,I16=16)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K15" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A15" s="3">
+      <c r="N15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="3">
         <f>'Win probabilities'!G8</f>
         <v>0.18390650213337789</v>
       </c>
-      <c r="C15" s="6">
-        <f ca="1">IF(RAND()&lt;A15,A14,A16)</f>
+      <c r="B16" s="11"/>
+      <c r="C16" s="5">
+        <f ca="1">IF(RAND()&lt;A16,A15,A17)</f>
         <v>7</v>
       </c>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="4">
+      <c r="E16" s="10" t="str">
+        <f ca="1">IF(B22=TRUE,'Win probabilities'!D6,"")</f>
+        <v/>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="10" t="str">
+        <f ca="1">IF(I22=TRUE,'Win probabilities'!L14,"")</f>
+        <v/>
+      </c>
+      <c r="I16" s="5">
+        <f ca="1">IF(RAND()&lt;K16,K15,K17)</f>
+        <v>15</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="3">
+        <f>'Win probabilities'!O16</f>
+        <v>0.38692769695651974</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="4">
         <v>8</v>
       </c>
-      <c r="C16" s="3" t="b">
-        <f ca="1">AND(C11=6,C15=8)</f>
+      <c r="B17" s="11" t="b">
+        <f ca="1">AND(C12=6,C16=8)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="3" t="b">
-        <f ca="1">IF(C16=TRUE,'Win probabilities'!F8)</f>
+      <c r="C17" s="3" t="str">
+        <f ca="1">IF(B17=TRUE,'Win probabilities'!F8," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E17" s="10" t="str">
+        <f ca="1">IF(C22=TRUE,'Win probabilities'!D7,"")</f>
+        <v/>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="10" t="str">
+        <f ca="1">IF(J22=TRUE,'Win probabilities'!L15,"")</f>
+        <v/>
+      </c>
+      <c r="I17" s="3" t="str">
+        <f ca="1">IF(J17=TRUE,'Win probabilities'!N16," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J17" s="11" t="b">
+        <f ca="1">AND(I12=14,I16=16)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K17" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="17" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="18" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="E18" s="10" t="str">
+        <f ca="1">IF(D22=TRUE,'Win probabilities'!D8,"")</f>
+        <v/>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="10" t="str">
+        <f ca="1">IF(K22=TRUE,'Win probabilities'!L16,"")</f>
+        <v/>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="13" t="b">
+        <f ca="1">AND($E$5=1,$E$14=5)</f>
+        <v>0</v>
+      </c>
+      <c r="B19" s="13" t="b">
+        <f ca="1">AND($E$5=1,$E$14=6)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="13" t="b">
+        <f ca="1">AND($E$5=1,$E$14=7)</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="13" t="b">
+        <f ca="1">AND($E$5=1,$E$14=8)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="13" t="b">
+        <f ca="1">AND(G5=9,G14=13)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="13" t="b">
+        <f ca="1">AND(G5=9,G14=14)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="13" t="b">
+        <f ca="1">AND(G5=9,G14=15)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="13" t="b">
+        <f ca="1">AND(G5=9,G14=16)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A20" s="13" t="b">
+        <f ca="1">AND($E$5=2,$E$14=5)</f>
+        <v>0</v>
+      </c>
+      <c r="B20" s="13" t="b">
+        <f ca="1">AND($E$5=2,$E$14=6)</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="13" t="b">
+        <f ca="1">AND($E$5=2,$E$14=7)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="13" t="b">
+        <f ca="1">AND($E$5=2,$E$14=8)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="13" t="b">
+        <f ca="1">AND(G5=10,G14=13)</f>
+        <v>1</v>
+      </c>
+      <c r="I20" s="13" t="b">
+        <f ca="1">AND(G5=10,G14=14)</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="13" t="b">
+        <f ca="1">AND(G5=10,G14=15)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="13" t="b">
+        <f ca="1">AND(G5=10,G14=16)</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A21" s="13" t="b">
+        <f ca="1">AND($E$5=3,$E$14=5)</f>
+        <v>0</v>
+      </c>
+      <c r="B21" s="13" t="b">
+        <f ca="1">AND($E$5=3,$E$14=6)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="13" t="b">
+        <f ca="1">AND($E$5=3,$E$14=7)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="13" t="b">
+        <f ca="1">AND($E$5=3,$E$14=8)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="13" t="b">
+        <f ca="1">AND(G5=11,G14=13)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="13" t="b">
+        <f ca="1">AND(G5=11,G14=14)</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="13" t="b">
+        <f ca="1">AND(G5=11,G14=15)</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="13" t="b">
+        <f ca="1">AND(G5=11,G14=16)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A22" s="13" t="b">
+        <f ca="1">AND($E$5=4,$E$14=5)</f>
+        <v>0</v>
+      </c>
+      <c r="B22" s="13" t="b">
+        <f ca="1">AND($E$5=4,$E$14=6)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="13" t="b">
+        <f ca="1">AND($E$5=4,$E$14=7)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="13" t="b">
+        <f ca="1">AND($E$5=4,$E$14=8)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="13" t="b">
+        <f ca="1">AND(G5=12,G14=13)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="13" t="b">
+        <f ca="1">AND(G5=12,G14=14)</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="13" t="b">
+        <f ca="1">AND(G5=12,G14=15)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="13" t="b">
+        <f ca="1">AND(G5=12,G14=16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I29" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I32" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -4134,6 +4833,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4421,15 +5129,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4451,6 +5150,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A33AA7F4-51CC-46CE-816E-9CAB67B26DBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F291531A-8552-416A-951C-C6D10D48BDBD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4471,14 +5178,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A33AA7F4-51CC-46CE-816E-9CAB67B26DBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89BFA361-931E-4B88-854C-2477F4226589}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Brian and Fraser modified visualization to protect cells
</commit_message>
<xml_diff>
--- a/visualization_wip.xlsx
+++ b/visualization_wip.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A527BC91-6B1C-4AD0-91A3-639E31460357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A96A45-A08B-4C91-84C2-F2143855C7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="533" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="533" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="START" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="5">
   <si>
     <t>ABOUT THIS TEMPLATE</t>
   </si>
@@ -61,7 +61,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -107,15 +107,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="24"/>
-      <color theme="0" tint="-0.14999847407452621"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.14999847407452621"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,23 +211,11 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
@@ -243,15 +224,47 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -373,8 +386,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2106962" y="713009"/>
-          <a:ext cx="1220653" cy="997527"/>
+          <a:off x="2148526" y="710700"/>
+          <a:ext cx="1248362" cy="992909"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="67" cy="204"/>
         </a:xfrm>
@@ -534,8 +547,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5404260" y="1242897"/>
-          <a:ext cx="1384467" cy="1981639"/>
+          <a:off x="5473533" y="1238279"/>
+          <a:ext cx="1444503" cy="1972402"/>
           <a:chOff x="460" y="254"/>
           <a:chExt cx="69" cy="408"/>
         </a:xfrm>
@@ -866,8 +879,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10986656" y="2493818"/>
-          <a:ext cx="1074950" cy="3990109"/>
+          <a:off x="11199092" y="2482273"/>
+          <a:ext cx="1074950" cy="3971636"/>
           <a:chOff x="655" y="467"/>
           <a:chExt cx="42" cy="848"/>
         </a:xfrm>
@@ -1023,8 +1036,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2105891" y="2750054"/>
-          <a:ext cx="1228726" cy="997527"/>
+          <a:off x="2147455" y="2738509"/>
+          <a:ext cx="1256435" cy="992909"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="65" cy="204"/>
         </a:xfrm>
@@ -1184,8 +1197,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2115416" y="5216236"/>
-          <a:ext cx="1209675" cy="1021274"/>
+          <a:off x="2156980" y="5193145"/>
+          <a:ext cx="1237384" cy="1016656"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="62" cy="204"/>
         </a:xfrm>
@@ -1345,8 +1358,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2115415" y="7252342"/>
-          <a:ext cx="1223354" cy="997527"/>
+          <a:off x="2156979" y="7220015"/>
+          <a:ext cx="1251063" cy="992909"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="64" cy="204"/>
         </a:xfrm>
@@ -1506,8 +1519,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="16495200" y="5216236"/>
-          <a:ext cx="1220263" cy="1065410"/>
+          <a:off x="16818473" y="5193145"/>
+          <a:ext cx="1238735" cy="1060792"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="64" cy="204"/>
         </a:xfrm>
@@ -1667,8 +1680,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="16500324" y="7252343"/>
-          <a:ext cx="1201724" cy="997527"/>
+          <a:off x="16823597" y="7220016"/>
+          <a:ext cx="1220196" cy="992909"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="63" cy="204"/>
         </a:xfrm>
@@ -1828,8 +1841,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16487902" y="755000"/>
-          <a:ext cx="1204357" cy="997527"/>
+          <a:off x="16811175" y="752691"/>
+          <a:ext cx="1222829" cy="992909"/>
           <a:chOff x="861" y="153"/>
           <a:chExt cx="60" cy="204"/>
         </a:xfrm>
@@ -1989,8 +2002,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16499604" y="2763469"/>
-          <a:ext cx="1139546" cy="997527"/>
+          <a:off x="16822877" y="2751924"/>
+          <a:ext cx="1139546" cy="992909"/>
           <a:chOff x="856" y="153"/>
           <a:chExt cx="65" cy="204"/>
         </a:xfrm>
@@ -2150,8 +2163,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5463886" y="5743575"/>
-          <a:ext cx="1334191" cy="1995055"/>
+          <a:off x="5572414" y="5718175"/>
+          <a:ext cx="1354972" cy="1985818"/>
           <a:chOff x="333" y="153"/>
           <a:chExt cx="64" cy="204"/>
         </a:xfrm>
@@ -2311,8 +2324,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13023273" y="1273752"/>
-          <a:ext cx="1357745" cy="1976005"/>
+          <a:off x="13277273" y="1269134"/>
+          <a:ext cx="1385454" cy="1966768"/>
           <a:chOff x="861" y="153"/>
           <a:chExt cx="60" cy="204"/>
         </a:xfrm>
@@ -2472,8 +2485,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13023273" y="5762625"/>
-          <a:ext cx="1357745" cy="1976005"/>
+          <a:off x="13277273" y="5737225"/>
+          <a:ext cx="1385454" cy="1966768"/>
           <a:chOff x="861" y="153"/>
           <a:chExt cx="60" cy="204"/>
         </a:xfrm>
@@ -3090,26 +3103,26 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="82.109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="2.77734375" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="8.77734375" style="8"/>
+    <col min="1" max="1" width="2.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="82.08984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="2.81640625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3128,1421 +3141,1687 @@
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.88671875" defaultRowHeight="39.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="16.90625" defaultRowHeight="39.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="30.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="30.77734375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="16.88671875" style="1"/>
+    <col min="1" max="1" width="30.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.90625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="30.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.54296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="30.81640625" style="1" customWidth="1"/>
+    <col min="12" max="15" width="16.90625" style="19"/>
+    <col min="16" max="16384" width="16.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="10"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="12" t="str">
+    <row r="1" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="15"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="7" t="str">
         <f ca="1">IF(A19=TRUE,'Win probabilities'!A5,"")</f>
         <v/>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="12" t="str">
+      <c r="F1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="str">
         <f ca="1">IF(H19=TRUE,'Win probabilities'!I13,"")</f>
         <v/>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
     </row>
-    <row r="2" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="4">
+    <row r="2" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="b">
+      <c r="B2" s="10" t="b">
         <f ca="1">AND(C3=A2,C7=A6)</f>
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="str">
+      <c r="C2" s="10" t="str">
         <f ca="1">IF(B2=TRUE,'Win probabilities'!A3," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E2" s="12" t="str">
+      <c r="D2" s="6"/>
+      <c r="E2" s="7" t="str">
         <f ca="1">IF(B19=TRUE,'Win probabilities'!A6,"")</f>
         <v/>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="12" t="str">
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="str">
         <f ca="1">IF(I19=TRUE,'Win probabilities'!I14,"")</f>
         <v/>
       </c>
-      <c r="I2" s="11" t="str">
+      <c r="H2" s="6"/>
+      <c r="I2" s="10" t="str">
         <f ca="1">IF(J2=TRUE,'Win probabilities'!I11," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J2" s="11" t="b">
+      <c r="J2" s="10" t="b">
         <f ca="1">AND(I3=K2,I7=K6)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="16">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="L2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="3">
+    <row r="3" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A3" s="6">
         <f>'Win probabilities'!A2</f>
         <v>0.98278630377518839</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="5">
+      <c r="B3" s="10"/>
+      <c r="C3" s="11">
         <f ca="1">IF(RAND()&lt;A3,A2,A4)</f>
         <v>1</v>
       </c>
-      <c r="E3" s="12" t="str">
+      <c r="D3" s="6"/>
+      <c r="E3" s="7" t="str">
         <f ca="1">IF(C19=TRUE,'Win probabilities'!A7,"")</f>
         <v/>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="12" t="str">
+      <c r="F3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7" t="str">
         <f ca="1">IF(J19=TRUE,'Win probabilities'!I15,"")</f>
         <v/>
       </c>
-      <c r="I3" s="5">
+      <c r="H3" s="6"/>
+      <c r="I3" s="11">
         <f ca="1">IF(RAND()&lt;K3,K2,K4)</f>
         <v>10</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="3">
+      <c r="J3" s="10"/>
+      <c r="K3" s="6">
         <f>'Win probabilities'!I10</f>
         <v>0.39616573899800145</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="L3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="20"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
     </row>
-    <row r="4" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="4">
+    <row r="4" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="b">
+      <c r="B4" s="10" t="b">
         <f ca="1">AND(C3=A4,C7=A6)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="11" t="str">
+      <c r="C4" s="10" t="str">
         <f ca="1">IF(B4=TRUE,'Win probabilities'!B3," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E4" s="12" t="str">
+      <c r="D4" s="6"/>
+      <c r="E4" s="7">
         <f ca="1">IF(D19=TRUE,'Win probabilities'!A8,"")</f>
-        <v/>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="12" t="str">
+        <v>0.58523501761644969</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7" t="str">
         <f ca="1">IF(K19=TRUE,'Win probabilities'!I16,"")</f>
         <v/>
       </c>
-      <c r="I4" s="11">
+      <c r="H4" s="6"/>
+      <c r="I4" s="10" t="str">
         <f ca="1">IF(J4=TRUE,'Win probabilities'!J11," ")</f>
-        <v>0.22852013706725405</v>
-      </c>
-      <c r="J4" s="11" t="b">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J4" s="10" t="b">
         <f ca="1">AND(I3=K4,I7=K6)</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="16">
         <v>10</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="L4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="20"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B5" s="11"/>
-      <c r="C5" s="3">
+    <row r="5" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A5" s="6"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="6">
         <f ca="1">SUM(C2,C4,C6,C8)</f>
         <v>0.73397479367659013</v>
       </c>
-      <c r="E5" s="6">
+      <c r="D5" s="6"/>
+      <c r="E5" s="12">
         <f ca="1">IF(RAND()&lt;SUM(C2,C4,C6,C8),C3,C7)</f>
-        <v>4</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="12">
         <f ca="1">IF(RAND()&lt;SUM(I2,I4,I6,I8),I3,I7)</f>
-        <v>11</v>
-      </c>
-      <c r="I5" s="3">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6">
         <f ca="1">SUM(I2,I4,I6,I8)</f>
-        <v>0.22852013706725405</v>
-      </c>
-      <c r="J5" s="11"/>
-      <c r="L5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>3</v>
-      </c>
+        <v>0.45256965598969556</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A6" s="4">
-        <v>3</v>
-      </c>
-      <c r="B6" s="11" t="b">
+    <row r="6" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A6" s="16">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10" t="b">
         <f ca="1">AND(C3=A2,C7=A8)</f>
         <v>1</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <f ca="1">IF(B6=TRUE,'Win probabilities'!A4," ")</f>
         <v>0.73397479367659013</v>
       </c>
-      <c r="E6" s="12" t="str">
+      <c r="D6" s="6"/>
+      <c r="E6" s="7" t="str">
         <f ca="1">IF(A20=TRUE,'Win probabilities'!B5,"")</f>
         <v/>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="12" t="str">
+      <c r="F6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="7">
         <f ca="1">IF(H20=TRUE,'Win probabilities'!J13,"")</f>
-        <v/>
-      </c>
-      <c r="I6" s="11" t="str">
+        <v>0.51246898889277914</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="10" t="str">
         <f ca="1">IF(J6=TRUE,'Win probabilities'!I12," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J6" s="11" t="b">
+      <c r="J6" s="10" t="b">
         <f ca="1">AND(I3=K2,I7=K8)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="16">
         <v>11</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="L6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A7" s="3">
+    <row r="7" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="6">
         <f>'Win probabilities'!C4</f>
         <v>0.60284487256253583</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="5">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11">
         <f ca="1">IF(RAND()&lt;A7,A6,A8)</f>
         <v>4</v>
       </c>
-      <c r="E7" s="12" t="str">
+      <c r="D7" s="6"/>
+      <c r="E7" s="7" t="str">
         <f ca="1">IF(B20=TRUE,'Win probabilities'!B6,"")</f>
         <v/>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <f ca="1">IF(RAND()&lt;F10,F9,F11)</f>
-        <v>5</v>
-      </c>
-      <c r="G7" s="12" t="str">
+        <v>13</v>
+      </c>
+      <c r="G7" s="7" t="str">
         <f ca="1">IF(I20=TRUE,'Win probabilities'!J14,"")</f>
         <v/>
       </c>
-      <c r="I7" s="5">
+      <c r="H7" s="6"/>
+      <c r="I7" s="11">
         <f ca="1">IF(RAND()&lt;K7,K6,K8)</f>
-        <v>11</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="3">
+        <v>12</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="6">
         <f>'Win probabilities'!K12</f>
         <v>0.4483559984872707</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="L7" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="20"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A8" s="4">
+    <row r="8" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A8" s="16">
         <v>4</v>
       </c>
-      <c r="B8" s="11" t="b">
+      <c r="B8" s="10" t="b">
         <f ca="1">AND(C3=A4,C7=A8)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="11" t="str">
+      <c r="C8" s="10" t="str">
         <f ca="1">IF(B8=TRUE,'Win probabilities'!B4," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E8" s="12" t="str">
+      <c r="D8" s="6"/>
+      <c r="E8" s="7" t="str">
         <f ca="1">IF(C20=TRUE,'Win probabilities'!B7,"")</f>
         <v/>
       </c>
-      <c r="G8" s="12" t="str">
+      <c r="F8" s="6"/>
+      <c r="G8" s="7" t="str">
         <f ca="1">IF(J20=TRUE,'Win probabilities'!J15,"")</f>
         <v/>
       </c>
-      <c r="I8" s="11" t="str">
+      <c r="H8" s="6"/>
+      <c r="I8" s="10">
         <f ca="1">IF(J8=TRUE,'Win probabilities'!J12," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="J8" s="11" t="b">
+        <v>0.45256965598969556</v>
+      </c>
+      <c r="J8" s="10" t="b">
         <f ca="1">AND(I3=K4,I7=K8)</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="16">
         <v>12</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="L8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="20"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B9" s="11"/>
-      <c r="D9" s="3">
+    <row r="9" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A9" s="6"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6">
         <f ca="1">SUM(E1:E4,E6:E13,E15:E18)</f>
-        <v>0.58979174292751868</v>
-      </c>
-      <c r="E9" s="12" t="str">
+        <v>0.58523501761644969</v>
+      </c>
+      <c r="E9" s="7" t="str">
         <f ca="1">IF(D20=TRUE,'Win probabilities'!B8,"")</f>
         <v/>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="13">
         <f ca="1">IF(RAND()&lt;SUM(E1:E4,E6:E13,E15:E18),E5,E14)</f>
-        <v>5</v>
-      </c>
-      <c r="G9" s="12" t="str">
+        <v>8</v>
+      </c>
+      <c r="G9" s="7" t="str">
         <f ca="1">IF(K20=TRUE,'Win probabilities'!J16,"")</f>
         <v/>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="6">
         <f ca="1">SUM(G1:G4,G6:G13,G15:G18)</f>
-        <v>0.51946314187411646</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="O9" s="3" t="s">
-        <v>3</v>
-      </c>
+        <v>0.51246898889277914</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
     </row>
-    <row r="10" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B10" s="11"/>
-      <c r="E10" s="12" t="str">
+    <row r="10" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A10" s="6"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7" t="str">
         <f ca="1">IF(A21=TRUE,'Win probabilities'!C5,"")</f>
         <v/>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="6">
         <f ca="1">SUM(A33:H40)</f>
-        <v>0.72885978719765732</v>
-      </c>
-      <c r="G10" s="12" t="str">
+        <v>2.2172095415460502E-2</v>
+      </c>
+      <c r="G10" s="7" t="str">
         <f ca="1">IF(H21=TRUE,'Win probabilities'!K13,"")</f>
         <v/>
       </c>
-      <c r="J10" s="11"/>
-      <c r="N10" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="20"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:16" s="3" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A11" s="4">
+    <row r="11" spans="1:18" s="3" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A11" s="16">
         <v>5</v>
       </c>
-      <c r="B11" s="11" t="b">
+      <c r="B11" s="10" t="b">
         <f ca="1">AND(C12=A11,C16=A15)</f>
-        <v>1</v>
-      </c>
-      <c r="C11" s="11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10" t="str">
         <f ca="1">IF(B11=TRUE,'Win probabilities'!E7," ")</f>
-        <v>0.27960125734444374</v>
-      </c>
-      <c r="E11" s="12" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7" t="str">
         <f ca="1">IF(B21=TRUE,'Win probabilities'!C6,"")</f>
         <v/>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="13">
         <f ca="1">IF(RAND()&lt;SUM(G1:G4,G6:G13,G15:G18),G5,G14)</f>
-        <v>11</v>
-      </c>
-      <c r="G11" s="12" t="str">
+        <v>13</v>
+      </c>
+      <c r="G11" s="7" t="str">
         <f ca="1">IF(I21=TRUE,'Win probabilities'!K14,"")</f>
         <v/>
       </c>
-      <c r="I11" s="11" t="str">
+      <c r="H11" s="6"/>
+      <c r="I11" s="10">
         <f ca="1">IF(J11=TRUE,'Win probabilities'!M15," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="J11" s="11" t="b">
+        <v>0.7109082374162673</v>
+      </c>
+      <c r="J11" s="10" t="b">
         <f ca="1">AND(I12=K11,I16=K15)</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="16">
         <v>13</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20" t="s">
         <v>4</v>
       </c>
+      <c r="O11" s="20"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="3">
+    <row r="12" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A12" s="6">
         <f>'Win probabilities'!E6</f>
         <v>0.99337376369869701</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="5">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11">
         <f ca="1">IF(RAND()&lt;A12,A11,A13)</f>
         <v>5</v>
       </c>
-      <c r="E12" s="12" t="str">
+      <c r="D12" s="6"/>
+      <c r="E12" s="7" t="str">
         <f ca="1">IF(C21=TRUE,'Win probabilities'!C7,"")</f>
         <v/>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="12" t="str">
+      <c r="F12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="7" t="str">
         <f ca="1">IF(J21=TRUE,'Win probabilities'!K15,"")</f>
         <v/>
       </c>
-      <c r="I12" s="5">
+      <c r="H12" s="6"/>
+      <c r="I12" s="11">
         <f ca="1">IF(RAND()&lt;K12,K11,K13)</f>
         <v>13</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="3">
+      <c r="J12" s="10"/>
+      <c r="K12" s="6">
         <f>'Win probabilities'!M14</f>
         <v>0.58056027074821481</v>
       </c>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A13" s="4">
+    <row r="13" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A13" s="16">
         <v>6</v>
       </c>
-      <c r="B13" s="11" t="b">
+      <c r="B13" s="10" t="b">
         <f ca="1">AND(C12=A13,C16=A15)</f>
         <v>0</v>
       </c>
-      <c r="C13" s="11" t="str">
+      <c r="C13" s="10" t="str">
         <f ca="1">IF(B13=TRUE,'Win probabilities'!F7," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E13" s="12" t="str">
+      <c r="D13" s="6"/>
+      <c r="E13" s="7" t="str">
         <f ca="1">IF(D21=TRUE,'Win probabilities'!C8,"")</f>
         <v/>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="12">
+      <c r="F13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="7" t="str">
         <f ca="1">IF(K21=TRUE,'Win probabilities'!K16,"")</f>
-        <v>0.51946314187411646</v>
-      </c>
-      <c r="I13" s="11" t="str">
+        <v/>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="10" t="str">
         <f ca="1">IF(J13=TRUE,'Win probabilities'!N15," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J13" s="11" t="b">
+      <c r="J13" s="10" t="b">
         <f ca="1">AND(I12=K13,I16=K15)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="16">
         <v>14</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" s="20"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B14" s="11"/>
-      <c r="C14" s="3">
+    <row r="14" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A14" s="6"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="6">
         <f ca="1">SUM(C11,C13,C15,C17)</f>
-        <v>0.27960125734444374</v>
-      </c>
-      <c r="E14" s="6">
+        <v>0.39975845501629426</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="12">
         <f ca="1">IF(RAND()&lt;SUM(C11,C13,C15,C17),C12,C16)</f>
-        <v>5</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="6">
+        <v>8</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="12">
         <f ca="1">IF(RAND()&lt;SUM(I11,I13,I15,I17),I12,I16)</f>
-        <v>16</v>
-      </c>
-      <c r="I14" s="3">
+        <v>13</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
         <f ca="1">SUM(I11,I13,I15,I17)</f>
-        <v>0.22010845846766691</v>
-      </c>
-      <c r="J14" s="11"/>
-      <c r="N14" s="3" t="s">
-        <v>3</v>
-      </c>
+        <v>0.7109082374162673</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="20"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A15" s="4">
+    <row r="15" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A15" s="16">
         <v>7</v>
       </c>
-      <c r="B15" s="11" t="b">
+      <c r="B15" s="10" t="b">
         <f ca="1">AND(C12=A11,C16=A17)</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="11" t="str">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10">
         <f ca="1">IF(B15=TRUE,'Win probabilities'!E8," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E15" s="12">
+        <v>0.39975845501629426</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7" t="str">
         <f ca="1">IF(A22=TRUE,'Win probabilities'!D5,"")</f>
-        <v>0.58979174292751868</v>
-      </c>
-      <c r="F15" s="12" t="str">
+        <v/>
+      </c>
+      <c r="F15" s="7" t="str">
         <f ca="1">IF(B22=TRUE,'Win probabilities'!E5,"")</f>
         <v/>
       </c>
-      <c r="G15" s="12" t="str">
+      <c r="G15" s="7" t="str">
         <f ca="1">IF(H22=TRUE,'Win probabilities'!L13,"")</f>
         <v/>
       </c>
-      <c r="I15" s="11">
+      <c r="H15" s="6"/>
+      <c r="I15" s="10" t="str">
         <f ca="1">IF(J15=TRUE,'Win probabilities'!M16," ")</f>
-        <v>0.22010845846766691</v>
-      </c>
-      <c r="J15" s="11" t="b">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J15" s="10" t="b">
         <f ca="1">AND(I12=K11,I16=K17)</f>
-        <v>1</v>
-      </c>
-      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="16">
         <v>15</v>
       </c>
-      <c r="N15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="20"/>
+      <c r="P15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:16" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="3">
+    <row r="16" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A16" s="6">
         <f>'Win probabilities'!G8</f>
         <v>0.18390650213337789</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="5">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11">
         <f ca="1">IF(RAND()&lt;A16,A15,A17)</f>
-        <v>7</v>
-      </c>
-      <c r="E16" s="12" t="str">
+        <v>8</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7" t="str">
         <f ca="1">IF(B22=TRUE,'Win probabilities'!D6,"")</f>
         <v/>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="12" t="str">
+      <c r="F16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="7" t="str">
         <f ca="1">IF(I22=TRUE,'Win probabilities'!L14,"")</f>
         <v/>
       </c>
-      <c r="I16" s="5">
+      <c r="H16" s="6"/>
+      <c r="I16" s="11">
         <f ca="1">IF(RAND()&lt;K16,K15,K17)</f>
-        <v>16</v>
-      </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="3">
+        <v>15</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="6">
         <f>'Win probabilities'!O16</f>
         <v>0.38692769695651974</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" s="20"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A17" s="4">
+    <row r="17" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A17" s="16">
         <v>8</v>
       </c>
-      <c r="B17" s="11" t="b">
+      <c r="B17" s="10" t="b">
         <f ca="1">AND(C12=A13,C16=A17)</f>
         <v>0</v>
       </c>
-      <c r="C17" s="11" t="str">
+      <c r="C17" s="10" t="str">
         <f ca="1">IF(B17=TRUE,'Win probabilities'!F8," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E17" s="12" t="str">
+      <c r="D17" s="6"/>
+      <c r="E17" s="7" t="str">
         <f ca="1">IF(C22=TRUE,'Win probabilities'!D7,"")</f>
         <v/>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="12" t="str">
+      <c r="F17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="7" t="str">
         <f ca="1">IF(J22=TRUE,'Win probabilities'!L15,"")</f>
         <v/>
       </c>
-      <c r="I17" s="11" t="str">
+      <c r="H17" s="6"/>
+      <c r="I17" s="10" t="str">
         <f ca="1">IF(J17=TRUE,'Win probabilities'!N16," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J17" s="11" t="b">
+      <c r="J17" s="10" t="b">
         <f ca="1">AND(I12=K13,I16=K17)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="16">
         <v>16</v>
       </c>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="E18" s="12" t="str">
+    <row r="18" spans="1:18" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7" t="str">
         <f ca="1">IF(D22=TRUE,'Win probabilities'!D8,"")</f>
         <v/>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="12" t="str">
+      <c r="F18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="7" t="str">
         <f ca="1">IF(K22=TRUE,'Win probabilities'!L16,"")</f>
         <v/>
       </c>
-      <c r="N18" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O18" s="20"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="13" t="b">
+    <row r="19" spans="1:18" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A19" s="17" t="b">
         <f ca="1">AND($E$5=A2,$E$14=A11)</f>
         <v>0</v>
       </c>
-      <c r="B19" s="13" t="b">
+      <c r="B19" s="17" t="b">
         <f ca="1">AND($E$5=A2,$E$14=A13)</f>
         <v>0</v>
       </c>
-      <c r="C19" s="13" t="b">
+      <c r="C19" s="17" t="b">
         <f ca="1">AND($E$5=A2,$E$14=A15)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="13" t="b">
+      <c r="D19" s="17" t="b">
         <f ca="1">AND($E$5=A2,$E$14=A17)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="17" t="b">
         <f ca="1">AND(G5=K2,G14=K11)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="13" t="b">
+      <c r="I19" s="17" t="b">
         <f ca="1">AND(G5=K2,G14=K13)</f>
         <v>0</v>
       </c>
-      <c r="J19" s="13" t="b">
+      <c r="J19" s="17" t="b">
         <f ca="1">AND(G5=K2,G14=K15)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="13" t="b">
+      <c r="K19" s="17" t="b">
         <f ca="1">AND(G5=K2,G14=K17)</f>
         <v>0</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="21"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
     </row>
-    <row r="20" spans="1:18" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A20" s="13" t="b">
+    <row r="20" spans="1:18" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A20" s="17" t="b">
         <f ca="1">AND($E$5=A4,$E$14=A11)</f>
         <v>0</v>
       </c>
-      <c r="B20" s="13" t="b">
+      <c r="B20" s="17" t="b">
         <f ca="1">AND($E$5=A4,$E$14=A13)</f>
         <v>0</v>
       </c>
-      <c r="C20" s="13" t="b">
+      <c r="C20" s="17" t="b">
         <f ca="1">AND($E$5=A4,$E$14=A15)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="13" t="b">
+      <c r="D20" s="17" t="b">
         <f ca="1">AND($E$5=A4,$E$14=A17)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="13" t="b">
+      <c r="E20" s="17"/>
+      <c r="F20" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="17" t="b">
         <f ca="1">AND(G5=K4,G14=K11)</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="17" t="b">
         <f ca="1">AND(G5=K4,G14=K13)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="13" t="b">
+      <c r="J20" s="17" t="b">
         <f ca="1">AND(G5=K4,G14=K15)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="13" t="b">
+      <c r="K20" s="17" t="b">
         <f ca="1">AND(G5=K4,G14=K17)</f>
         <v>0</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="R20" s="2" t="s">
+      <c r="L20" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O20" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R20" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A21" s="13" t="b">
+    <row r="21" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A21" s="17" t="b">
         <f ca="1">AND($E$5=A6,$E$14=A11)</f>
         <v>0</v>
       </c>
-      <c r="B21" s="13" t="b">
+      <c r="B21" s="17" t="b">
         <f ca="1">AND($E$5=A6,$E$14=A13)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="13" t="b">
+      <c r="C21" s="17" t="b">
         <f ca="1">AND($E$5=A6,$E$14=A15)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="13" t="b">
+      <c r="D21" s="17" t="b">
         <f ca="1">AND($E$5=A6,$E$14=A17)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H21" s="13" t="b">
+      <c r="E21" s="17"/>
+      <c r="F21" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="17" t="b">
         <f ca="1">AND(G5=K6,G14=K11)</f>
         <v>0</v>
       </c>
-      <c r="I21" s="13" t="b">
+      <c r="I21" s="17" t="b">
         <f ca="1">AND(G5=K6,G14=K13)</f>
         <v>0</v>
       </c>
-      <c r="J21" s="13" t="b">
+      <c r="J21" s="17" t="b">
         <f ca="1">AND(G5=K6,G14=K15)</f>
         <v>0</v>
       </c>
-      <c r="K21" s="13" t="b">
+      <c r="K21" s="17" t="b">
         <f ca="1">AND(G5=K6,G14=K17)</f>
-        <v>1</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
     </row>
-    <row r="22" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="13" t="b">
+    <row r="22" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A22" s="17" t="b">
         <f ca="1">AND($E$5=A8,$E$14=A11)</f>
-        <v>1</v>
-      </c>
-      <c r="B22" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="B22" s="17" t="b">
         <f ca="1">AND($E$5=A8,$E$14=A13)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="13" t="b">
+      <c r="C22" s="17" t="b">
         <f ca="1">AND($E$5=A8,$E$14=A15)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="13" t="b">
+      <c r="D22" s="17" t="b">
         <f ca="1">AND($E$5=A8,$E$14=A17)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H22" s="13" t="b">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="17" t="b">
         <f ca="1">AND(G5=K8,G14=K11)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="13" t="b">
+      <c r="I22" s="17" t="b">
         <f ca="1">AND(G5=K8,G14=K13)</f>
         <v>0</v>
       </c>
-      <c r="J22" s="13" t="b">
+      <c r="J22" s="17" t="b">
         <f ca="1">AND(G5=K8,G14=K15)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="13" t="b">
+      <c r="K22" s="17" t="b">
         <f ca="1">AND(G5=K8,G14=K17)</f>
         <v>0</v>
       </c>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
     </row>
     <row r="23" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" s="18"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
     </row>
-    <row r="24" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="13" t="b">
+    <row r="24" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A24" s="17" t="b">
         <f ca="1">AND($F$9=A2,$F$11=K2)</f>
         <v>0</v>
       </c>
-      <c r="B24" s="13" t="b">
+      <c r="B24" s="17" t="b">
         <f ca="1">AND($F$9=A2,$F$11=K4)</f>
         <v>0</v>
       </c>
-      <c r="C24" s="13" t="b">
+      <c r="C24" s="17" t="b">
         <f ca="1">AND($F$9=A2,$F$11=K6)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="13" t="b">
+      <c r="D24" s="17" t="b">
         <f ca="1">AND($F$9=A2,$F$11=K8)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="13" t="b">
+      <c r="E24" s="17" t="b">
         <f ca="1">AND($F$9=A2,$F$11=K11)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="13" t="b">
+      <c r="F24" s="17" t="b">
         <f ca="1">AND($F$9=A2,$F$11=K13)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="13" t="b">
+      <c r="G24" s="17" t="b">
         <f ca="1">AND($F$9=A2,$F$11=K15)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="13" t="b">
+      <c r="H24" s="17" t="b">
         <f ca="1">AND($F$9=A2,$F$11=K17)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="13"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
     </row>
-    <row r="25" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A25" s="13" t="b">
+    <row r="25" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A25" s="17" t="b">
         <f ca="1">AND($F$9=A4,$F$11=K2)</f>
         <v>0</v>
       </c>
-      <c r="B25" s="13" t="b">
+      <c r="B25" s="17" t="b">
         <f ca="1">AND($F$9=A4,$F$11=K4)</f>
         <v>0</v>
       </c>
-      <c r="C25" s="13" t="b">
+      <c r="C25" s="17" t="b">
         <f ca="1">AND($F$9=A4,$F$11=K6)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="13" t="b">
+      <c r="D25" s="17" t="b">
         <f ca="1">AND($F$9=A4,$F$11=K8)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="13" t="b">
+      <c r="E25" s="17" t="b">
         <f ca="1">AND($F$9=A4,$F$11=K11)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="13" t="b">
+      <c r="F25" s="17" t="b">
         <f ca="1">AND($F$9=A4,$F$11=K13)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="13" t="b">
+      <c r="G25" s="17" t="b">
         <f ca="1">AND($F$9=A4,$F$11=K15)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="13" t="b">
+      <c r="H25" s="17" t="b">
         <f ca="1">AND($F$9=A4,$F$11=K17)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="I25" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="18"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
     </row>
-    <row r="26" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A26" s="13" t="b">
+    <row r="26" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A26" s="17" t="b">
         <f ca="1">AND($F$9=A6,$F$11=K2)</f>
         <v>0</v>
       </c>
-      <c r="B26" s="13" t="b">
+      <c r="B26" s="17" t="b">
         <f ca="1">AND($F$9=A6,$F$11=K4)</f>
         <v>0</v>
       </c>
-      <c r="C26" s="13" t="b">
+      <c r="C26" s="17" t="b">
         <f ca="1">AND($F$9=A6,$F$11=K6)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="13" t="b">
+      <c r="D26" s="17" t="b">
         <f ca="1">AND($F$9=A6,$F$11=K8)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="13" t="b">
+      <c r="E26" s="17" t="b">
         <f ca="1">AND($F$9=A6,$F$11=K11)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="13" t="b">
+      <c r="F26" s="17" t="b">
         <f ca="1">AND($F$9=A6,$F$11=K13)</f>
         <v>0</v>
       </c>
-      <c r="G26" s="13" t="b">
+      <c r="G26" s="17" t="b">
         <f ca="1">AND($F$9=A6,$F$11=K15)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="13" t="b">
+      <c r="H26" s="17" t="b">
         <f ca="1">AND($F$9=A6,$F$11=K17)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="I26" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
     </row>
-    <row r="27" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A27" s="13" t="b">
+    <row r="27" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A27" s="17" t="b">
         <f ca="1">AND($F$9=A8,$F$11=K2)</f>
         <v>0</v>
       </c>
-      <c r="B27" s="13" t="b">
+      <c r="B27" s="17" t="b">
         <f ca="1">AND($F$9=A8,$F$11=K4)</f>
         <v>0</v>
       </c>
-      <c r="C27" s="13" t="b">
+      <c r="C27" s="17" t="b">
         <f ca="1">AND($F$9=A8,$F$11=K6)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="13" t="b">
+      <c r="D27" s="17" t="b">
         <f ca="1">AND($F$9=A8,$F$11=K8)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="13" t="b">
+      <c r="E27" s="17" t="b">
         <f ca="1">AND($F$9=A8,$F$11=K11)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="13" t="b">
+      <c r="F27" s="17" t="b">
         <f ca="1">AND($F$9=A8,$F$11=K13)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="13" t="b">
+      <c r="G27" s="17" t="b">
         <f ca="1">AND($F$9=A8,$F$11=K15)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="13" t="b">
+      <c r="H27" s="17" t="b">
         <f ca="1">AND($F$9=A8,$F$11=K17)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="I27" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
     </row>
-    <row r="28" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="13" t="b">
+    <row r="28" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A28" s="17" t="b">
         <f ca="1">AND($F$9=A11,$F$11=K2)</f>
         <v>0</v>
       </c>
-      <c r="B28" s="13" t="b">
+      <c r="B28" s="17" t="b">
         <f ca="1">AND($F$9=A11,$F$11=K4)</f>
         <v>0</v>
       </c>
-      <c r="C28" s="13" t="b">
+      <c r="C28" s="17" t="b">
         <f ca="1">AND($F$9=A11,$F$11=K6)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="17" t="b">
+        <f ca="1">AND($F$9=A11,$F$11=K8)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="17" t="b">
+        <f ca="1">AND($F$9=A11,$F$11=K11)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="17" t="b">
+        <f ca="1">AND($F$9=A11,$F$11=K13)</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="17" t="b">
+        <f ca="1">AND($F$9=A11,$F$11=K15)</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="17" t="b">
+        <f ca="1">AND($F$9=A11,$F$11=K17)</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+    </row>
+    <row r="29" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A29" s="17" t="b">
+        <f ca="1">AND($F$9=A13,$F$11=K2)</f>
+        <v>0</v>
+      </c>
+      <c r="B29" s="17" t="b">
+        <f ca="1">AND($F$9=A13,$F$11=K4)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="17" t="b">
+        <f ca="1">AND($F$9=A13,$F$11=K6)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="17" t="b">
+        <f ca="1">AND($F$9=A13,$F$11=K8)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="17" t="b">
+        <f ca="1">AND($F$9=A13,$F$11=K11)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="17" t="b">
+        <f ca="1">AND($F$9=A13,$F$11=K13)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="17" t="b">
+        <f ca="1">AND($F$9=A13,$F$11=K15)</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="17" t="b">
+        <f ca="1">AND($F$9=A13,$F$11=K17)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+    </row>
+    <row r="30" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A30" s="17" t="b">
+        <f ca="1">AND($F$9=A15,$F$11=K2)</f>
+        <v>0</v>
+      </c>
+      <c r="B30" s="17" t="b">
+        <f ca="1">AND($F$9=A15,$F$11=K4)</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="17" t="b">
+        <f ca="1">AND($F$9=A15,$F$11=K6)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="17" t="b">
+        <f ca="1">AND($F$9=A15,$F$11=K8)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="17" t="b">
+        <f ca="1">AND($F$9=A15,$F$11=K11)</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="17" t="b">
+        <f ca="1">AND($F$9=A15,$F$11=K13)</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="17" t="b">
+        <f ca="1">AND($F$9=A15,$F$11=K15)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="17" t="b">
+        <f ca="1">AND($F$9=A15,$F$11=K17)</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+    </row>
+    <row r="31" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A31" s="17" t="b">
+        <f ca="1">AND($F$9=A17,$F$11=K2)</f>
+        <v>0</v>
+      </c>
+      <c r="B31" s="17" t="b">
+        <f ca="1">AND($F$9=A17,$F$11=K4)</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="17" t="b">
+        <f ca="1">AND($F$9=A17,$F$11=K6)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="17" t="b">
+        <f ca="1">AND($F$9=A17,$F$11=K8)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="17" t="b">
+        <f ca="1">AND($F$9=A17,$F$11=K11)</f>
         <v>1</v>
       </c>
-      <c r="D28" s="13" t="b">
-        <f ca="1">AND($F$9=A11,$F$11=K8)</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="13" t="b">
-        <f ca="1">AND($F$9=A11,$F$11=K11)</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="13" t="b">
-        <f ca="1">AND($F$9=A11,$F$11=K13)</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="13" t="b">
-        <f ca="1">AND($F$9=A11,$F$11=K15)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="13" t="b">
-        <f ca="1">AND($F$9=A11,$F$11=K17)</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A29" s="13" t="b">
-        <f ca="1">AND($F$9=A13,$F$11=K2)</f>
-        <v>0</v>
-      </c>
-      <c r="B29" s="13" t="b">
-        <f ca="1">AND($F$9=A13,$F$11=K4)</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="13" t="b">
-        <f ca="1">AND($F$9=A13,$F$11=K6)</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="13" t="b">
-        <f ca="1">AND($F$9=A13,$F$11=K8)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="13" t="b">
-        <f ca="1">AND($F$9=A13,$F$11=K11)</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="13" t="b">
-        <f ca="1">AND($F$9=A13,$F$11=K13)</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="13" t="b">
-        <f ca="1">AND($F$9=A13,$F$11=K15)</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="13" t="b">
-        <f ca="1">AND($F$9=A13,$F$11=K17)</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A30" s="13" t="b">
-        <f ca="1">AND($F$9=A15,$F$11=K2)</f>
-        <v>0</v>
-      </c>
-      <c r="B30" s="13" t="b">
-        <f ca="1">AND($F$9=A15,$F$11=K4)</f>
-        <v>0</v>
-      </c>
-      <c r="C30" s="13" t="b">
-        <f ca="1">AND($F$9=A15,$F$11=K6)</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="13" t="b">
-        <f ca="1">AND($F$9=A15,$F$11=K8)</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="13" t="b">
-        <f ca="1">AND($F$9=A15,$F$11=K11)</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="13" t="b">
-        <f ca="1">AND($F$9=A15,$F$11=K13)</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="13" t="b">
-        <f ca="1">AND($F$9=A15,$F$11=K15)</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="13" t="b">
-        <f ca="1">AND($F$9=A15,$F$11=K17)</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A31" s="13" t="b">
-        <f ca="1">AND($F$9=A17,$F$11=K2)</f>
-        <v>0</v>
-      </c>
-      <c r="B31" s="13" t="b">
-        <f ca="1">AND($F$9=A17,$F$11=K4)</f>
-        <v>0</v>
-      </c>
-      <c r="C31" s="13" t="b">
-        <f ca="1">AND($F$9=A17,$F$11=K6)</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="13" t="b">
-        <f ca="1">AND($F$9=A17,$F$11=K8)</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="13" t="b">
-        <f ca="1">AND($F$9=A17,$F$11=K11)</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="13" t="b">
+      <c r="F31" s="17" t="b">
         <f ca="1">AND($F$9=A17,$F$11=K13)</f>
         <v>0</v>
       </c>
-      <c r="G31" s="13" t="b">
+      <c r="G31" s="17" t="b">
         <f ca="1">AND($F$9=A17,$F$11=K15)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="13" t="b">
+      <c r="H31" s="17" t="b">
         <f ca="1">AND($F$9=A17,$F$11=K17)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="I31" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
     </row>
     <row r="32" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I32" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
     </row>
-    <row r="33" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A33" s="13" t="str">
+    <row r="33" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A33" s="17" t="str">
         <f ca="1">IF(A24=TRUE,'Win probabilities'!A9,"-")</f>
         <v>-</v>
       </c>
-      <c r="B33" s="13" t="str">
+      <c r="B33" s="17" t="str">
         <f ca="1">IF(B24=TRUE,'Win probabilities'!A10,"-")</f>
         <v>-</v>
       </c>
-      <c r="C33" s="13" t="str">
+      <c r="C33" s="17" t="str">
         <f ca="1">IF(C24=TRUE,'Win probabilities'!A11,"-")</f>
         <v>-</v>
       </c>
-      <c r="D33" s="13" t="str">
+      <c r="D33" s="17" t="str">
         <f ca="1">IF(D24=TRUE,'Win probabilities'!A12,"-")</f>
         <v>-</v>
       </c>
-      <c r="E33" s="13" t="str">
+      <c r="E33" s="17" t="str">
         <f ca="1">IF(E24=TRUE,'Win probabilities'!A13,"-")</f>
         <v>-</v>
       </c>
-      <c r="F33" s="13" t="str">
+      <c r="F33" s="17" t="str">
         <f ca="1">IF(F24=TRUE,'Win probabilities'!A14,"-")</f>
         <v>-</v>
       </c>
-      <c r="G33" s="13" t="str">
+      <c r="G33" s="17" t="str">
         <f ca="1">IF(G24=TRUE,'Win probabilities'!A15,"-")</f>
         <v>-</v>
       </c>
-      <c r="H33" s="13" t="str">
+      <c r="H33" s="17" t="str">
         <f ca="1">IF(H24=TRUE,'Win probabilities'!A16,"-")</f>
         <v>-</v>
       </c>
-      <c r="I33" s="14" t="s">
-        <v>3</v>
-      </c>
+      <c r="I33" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
     </row>
-    <row r="34" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A34" s="13" t="str">
+    <row r="34" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A34" s="17" t="str">
         <f ca="1">IF(A25=TRUE,'Win probabilities'!B9,"-")</f>
         <v>-</v>
       </c>
-      <c r="B34" s="13" t="str">
+      <c r="B34" s="17" t="str">
         <f ca="1">IF(B25=TRUE,'Win probabilities'!B10,"-")</f>
         <v>-</v>
       </c>
-      <c r="C34" s="13" t="str">
+      <c r="C34" s="17" t="str">
         <f ca="1">IF(C25=TRUE,'Win probabilities'!B11,"-")</f>
         <v>-</v>
       </c>
-      <c r="D34" s="13" t="str">
+      <c r="D34" s="17" t="str">
         <f ca="1">IF(D25=TRUE,'Win probabilities'!B12,"-")</f>
         <v>-</v>
       </c>
-      <c r="E34" s="13" t="str">
+      <c r="E34" s="17" t="str">
         <f ca="1">IF(E25=TRUE,'Win probabilities'!B13,"-")</f>
         <v>-</v>
       </c>
-      <c r="F34" s="13" t="str">
+      <c r="F34" s="17" t="str">
         <f ca="1">IF(F25=TRUE,'Win probabilities'!B14,"-")</f>
         <v>-</v>
       </c>
-      <c r="G34" s="13" t="str">
+      <c r="G34" s="17" t="str">
         <f ca="1">IF(G25=TRUE,'Win probabilities'!B15,"-")</f>
         <v>-</v>
       </c>
-      <c r="H34" s="13" t="str">
+      <c r="H34" s="17" t="str">
         <f ca="1">IF(H25=TRUE,'Win probabilities'!B16,"-")</f>
         <v>-</v>
       </c>
-      <c r="I34" s="14" t="s">
-        <v>3</v>
-      </c>
+      <c r="I34" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
     </row>
-    <row r="35" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="13" t="str">
+    <row r="35" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A35" s="17" t="str">
         <f ca="1">IF(A26=TRUE,'Win probabilities'!C9,"-")</f>
         <v>-</v>
       </c>
-      <c r="B35" s="13" t="str">
+      <c r="B35" s="17" t="str">
         <f ca="1">IF(B26=TRUE,'Win probabilities'!C10,"-")</f>
         <v>-</v>
       </c>
-      <c r="C35" s="13" t="str">
+      <c r="C35" s="17" t="str">
         <f ca="1">IF(C26=TRUE,'Win probabilities'!C11,"-")</f>
         <v>-</v>
       </c>
-      <c r="D35" s="13" t="str">
+      <c r="D35" s="17" t="str">
         <f ca="1">IF(D26=TRUE,'Win probabilities'!C12,"-")</f>
         <v>-</v>
       </c>
-      <c r="E35" s="13" t="str">
+      <c r="E35" s="17" t="str">
         <f ca="1">IF(E26=TRUE,'Win probabilities'!C13,"-")</f>
         <v>-</v>
       </c>
-      <c r="F35" s="13" t="str">
+      <c r="F35" s="17" t="str">
         <f ca="1">IF(F26=TRUE,'Win probabilities'!C14,"-")</f>
         <v>-</v>
       </c>
-      <c r="G35" s="13" t="str">
+      <c r="G35" s="17" t="str">
         <f ca="1">IF(G26=TRUE,'Win probabilities'!C15,"-")</f>
         <v>-</v>
       </c>
-      <c r="H35" s="13" t="str">
+      <c r="H35" s="17" t="str">
         <f ca="1">IF(H26=TRUE,'Win probabilities'!C16,"-")</f>
         <v>-</v>
       </c>
-      <c r="I35" s="14"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
     </row>
-    <row r="36" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A36" s="13" t="str">
+    <row r="36" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A36" s="17" t="str">
         <f ca="1">IF(A27=TRUE,'Win probabilities'!D9,"-")</f>
         <v>-</v>
       </c>
-      <c r="B36" s="13" t="str">
+      <c r="B36" s="17" t="str">
         <f ca="1">IF(B27=TRUE,'Win probabilities'!D10,"-")</f>
         <v>-</v>
       </c>
-      <c r="C36" s="13" t="str">
+      <c r="C36" s="17" t="str">
         <f ca="1">IF(C27=TRUE,'Win probabilities'!D11,"-")</f>
         <v>-</v>
       </c>
-      <c r="D36" s="13" t="str">
+      <c r="D36" s="17" t="str">
         <f ca="1">IF(D27=TRUE,'Win probabilities'!D12,"-")</f>
         <v>-</v>
       </c>
-      <c r="E36" s="13" t="str">
+      <c r="E36" s="17" t="str">
         <f ca="1">IF(E27=TRUE,'Win probabilities'!D13,"-")</f>
         <v>-</v>
       </c>
-      <c r="F36" s="13" t="str">
+      <c r="F36" s="17" t="str">
         <f ca="1">IF(F27=TRUE,'Win probabilities'!D14,"-")</f>
         <v>-</v>
       </c>
-      <c r="G36" s="13" t="str">
+      <c r="G36" s="17" t="str">
         <f ca="1">IF(G27=TRUE,'Win probabilities'!D15,"-")</f>
         <v>-</v>
       </c>
-      <c r="H36" s="13" t="str">
+      <c r="H36" s="17" t="str">
         <f ca="1">IF(H27=TRUE,'Win probabilities'!D16,"-")</f>
         <v>-</v>
       </c>
-      <c r="I36" s="14"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
     </row>
-    <row r="37" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="13" t="str">
+    <row r="37" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A37" s="17" t="str">
         <f ca="1">IF(A28=TRUE,'Win probabilities'!E9,"-")</f>
         <v>-</v>
       </c>
-      <c r="B37" s="13" t="str">
+      <c r="B37" s="17" t="str">
         <f ca="1">IF(B28=TRUE,'Win probabilities'!E10,"-")</f>
         <v>-</v>
       </c>
-      <c r="C37" s="13">
+      <c r="C37" s="17" t="str">
         <f ca="1">IF(C28=TRUE,'Win probabilities'!E11,"-")</f>
-        <v>0.72885978719765732</v>
-      </c>
-      <c r="D37" s="13" t="str">
+        <v>-</v>
+      </c>
+      <c r="D37" s="17" t="str">
         <f ca="1">IF(D28=TRUE,'Win probabilities'!E12,"-")</f>
         <v>-</v>
       </c>
-      <c r="E37" s="13" t="str">
+      <c r="E37" s="17" t="str">
         <f ca="1">IF(E28=TRUE,'Win probabilities'!E13,"-")</f>
         <v>-</v>
       </c>
-      <c r="F37" s="13" t="str">
+      <c r="F37" s="17" t="str">
         <f ca="1">IF(F28=TRUE,'Win probabilities'!E14,"-")</f>
         <v>-</v>
       </c>
-      <c r="G37" s="13" t="str">
+      <c r="G37" s="17" t="str">
         <f ca="1">IF(G28=TRUE,'Win probabilities'!E15,"-")</f>
         <v>-</v>
       </c>
-      <c r="H37" s="13" t="str">
+      <c r="H37" s="17" t="str">
         <f ca="1">IF(H28=TRUE,'Win probabilities'!E16,"-")</f>
         <v>-</v>
       </c>
-      <c r="I37" s="14"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
     </row>
-    <row r="38" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A38" s="13" t="str">
+    <row r="38" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A38" s="17" t="str">
         <f ca="1">IF(A29=TRUE,'Win probabilities'!F9,"-")</f>
         <v>-</v>
       </c>
-      <c r="B38" s="13" t="str">
+      <c r="B38" s="17" t="str">
         <f ca="1">IF(B29=TRUE,'Win probabilities'!F10,"-")</f>
         <v>-</v>
       </c>
-      <c r="C38" s="13" t="str">
+      <c r="C38" s="17" t="str">
         <f ca="1">IF(C29=TRUE,'Win probabilities'!F11,"-")</f>
         <v>-</v>
       </c>
-      <c r="D38" s="13" t="str">
+      <c r="D38" s="17" t="str">
         <f ca="1">IF(D29=TRUE,'Win probabilities'!F12,"-")</f>
         <v>-</v>
       </c>
-      <c r="E38" s="13" t="str">
+      <c r="E38" s="17" t="str">
         <f ca="1">IF(E29=TRUE,'Win probabilities'!F13,"-")</f>
         <v>-</v>
       </c>
-      <c r="F38" s="13" t="str">
+      <c r="F38" s="17" t="str">
         <f ca="1">IF(F29=TRUE,'Win probabilities'!F14,"-")</f>
         <v>-</v>
       </c>
-      <c r="G38" s="13" t="str">
+      <c r="G38" s="17" t="str">
         <f ca="1">IF(G29=TRUE,'Win probabilities'!F15,"-")</f>
         <v>-</v>
       </c>
-      <c r="H38" s="13" t="str">
+      <c r="H38" s="17" t="str">
         <f ca="1">IF(H29=TRUE,'Win probabilities'!F16,"-")</f>
         <v>-</v>
       </c>
-      <c r="I38" s="14"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
     </row>
-    <row r="39" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A39" s="13" t="str">
+    <row r="39" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A39" s="17" t="str">
         <f ca="1">IF(A30=TRUE,'Win probabilities'!G9,"-")</f>
         <v>-</v>
       </c>
-      <c r="B39" s="13" t="str">
+      <c r="B39" s="17" t="str">
         <f ca="1">IF(B30=TRUE,'Win probabilities'!G10,"-")</f>
         <v>-</v>
       </c>
-      <c r="C39" s="13" t="str">
+      <c r="C39" s="17" t="str">
         <f ca="1">IF(C30=TRUE,'Win probabilities'!G11,"-")</f>
         <v>-</v>
       </c>
-      <c r="D39" s="13" t="str">
+      <c r="D39" s="17" t="str">
         <f ca="1">IF(D30=TRUE,'Win probabilities'!G12,"-")</f>
         <v>-</v>
       </c>
-      <c r="E39" s="13" t="str">
+      <c r="E39" s="17" t="str">
         <f ca="1">IF(E30=TRUE,'Win probabilities'!G13,"-")</f>
         <v>-</v>
       </c>
-      <c r="F39" s="13" t="str">
+      <c r="F39" s="17" t="str">
         <f ca="1">IF(F30=TRUE,'Win probabilities'!G14,"-")</f>
         <v>-</v>
       </c>
-      <c r="G39" s="13" t="str">
+      <c r="G39" s="17" t="str">
         <f ca="1">IF(G30=TRUE,'Win probabilities'!G15,"-")</f>
         <v>-</v>
       </c>
-      <c r="H39" s="13" t="str">
+      <c r="H39" s="17" t="str">
         <f ca="1">IF(H30=TRUE,'Win probabilities'!G16,"-")</f>
         <v>-</v>
       </c>
-      <c r="I39" s="14"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
     </row>
-    <row r="40" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A40" s="13" t="str">
+    <row r="40" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A40" s="17" t="str">
         <f ca="1">IF(A31=TRUE,'Win probabilities'!H9,"-")</f>
         <v>-</v>
       </c>
-      <c r="B40" s="13" t="str">
+      <c r="B40" s="17" t="str">
         <f ca="1">IF(B31=TRUE,'Win probabilities'!H10,"-")</f>
         <v>-</v>
       </c>
-      <c r="C40" s="13" t="str">
+      <c r="C40" s="17" t="str">
         <f ca="1">IF(C31=TRUE,'Win probabilities'!H11,"-")</f>
         <v>-</v>
       </c>
-      <c r="D40" s="13" t="str">
+      <c r="D40" s="17" t="str">
         <f ca="1">IF(D31=TRUE,'Win probabilities'!H12,"-")</f>
         <v>-</v>
       </c>
-      <c r="E40" s="13" t="str">
+      <c r="E40" s="17">
         <f ca="1">IF(E31=TRUE,'Win probabilities'!H13,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="F40" s="13" t="str">
+        <v>2.2172095415460502E-2</v>
+      </c>
+      <c r="F40" s="17" t="str">
         <f ca="1">IF(F31=TRUE,'Win probabilities'!H14,"-")</f>
         <v>-</v>
       </c>
-      <c r="G40" s="13" t="str">
+      <c r="G40" s="17" t="str">
         <f ca="1">IF(G31=TRUE,'Win probabilities'!H15,"-")</f>
         <v>-</v>
       </c>
-      <c r="H40" s="13" t="str">
+      <c r="H40" s="17" t="str">
         <f ca="1">IF(H31=TRUE,'Win probabilities'!H16,"-")</f>
         <v>-</v>
       </c>
-      <c r="I40" s="14"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Mxgo852965PU4CtHWJ33aE1FZzN6O9DD+pSameFXiJiej7M5TQgUm2JuvGxKz40zMxOwu43+g5YUy6EUlqHHgA==" saltValue="p5i1MIU82YIGhDHQcJSkhw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="1" bottom="1" header="0.49" footer="0.5"/>
@@ -4560,7 +4839,7 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -5368,6 +5647,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5655,36 +5963,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89BFA361-931E-4B88-854C-2477F4226589}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A33AA7F4-51CC-46CE-816E-9CAB67B26DBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F291531A-8552-416A-951C-C6D10D48BDBD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5703,24 +6002,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A33AA7F4-51CC-46CE-816E-9CAB67B26DBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89BFA361-931E-4B88-854C-2477F4226589}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>